<commit_message>
Modificacion del Modelo entidad-relacion
</commit_message>
<xml_diff>
--- a/Requerimientos funcionales/Requerimientos Funcionales.xlsx
+++ b/Requerimientos funcionales/Requerimientos Funcionales.xlsx
@@ -246,9 +246,6 @@
     <t>4.4.1. Antes de efectuar la venta, se debe validar que la compra sea en efectivo o con tarjeta, esto para efectos de descuentos</t>
   </si>
   <si>
-    <t>4.4.2. Si es con tarjeta, se debe guardar en una base de datos el tipo de tarjeta con la que se esté pagando, el banco y los ultimos 6 números para tener un control en posteriores ventas</t>
-  </si>
-  <si>
     <t>4.5. Verificación de tipo de factura (Mayoreo o Detalle)</t>
   </si>
   <si>
@@ -283,13 +280,36 @@
   </si>
   <si>
     <t>3.5.3. El transporte del pedido debe agregarse según el tipo de proveedor, ya sea por encomienda o personalmente</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">4.4.2. Si es con tarjeta, se debe guardar en una base de datos el tipo de tarjeta con la que se esté pagando, el banco y los ultimos </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>4</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> números para tener un control en posteriores ventas</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -358,6 +378,12 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="5">
@@ -455,6 +481,20 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="justify" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
@@ -472,20 +512,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="justify" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -794,8 +820,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A5:AF175"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E63" sqref="E63:H63"/>
+    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
+      <selection activeCell="K58" sqref="K58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -886,16 +912,16 @@
       <c r="B8" s="4"/>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="8" t="s">
+      <c r="E8" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="10" t="s">
+      <c r="F8" s="16" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="12" t="s">
+      <c r="G8" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="H8" s="12" t="s">
+      <c r="H8" s="18" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="4"/>
@@ -928,10 +954,10 @@
       <c r="B9" s="4"/>
       <c r="C9" s="4"/>
       <c r="D9" s="4"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="E9" s="15"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="19"/>
+      <c r="H9" s="19"/>
       <c r="I9" s="4"/>
       <c r="J9" s="4"/>
       <c r="K9" s="4"/>
@@ -1004,16 +1030,16 @@
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
       <c r="D11" s="4"/>
-      <c r="E11" s="19" t="s">
+      <c r="E11" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F11" s="14" t="s">
+      <c r="F11" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="14" t="s">
+      <c r="G11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H11" s="14" t="s">
+      <c r="H11" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I11" s="4"/>
@@ -1041,63 +1067,63 @@
       <c r="AE11" s="4"/>
       <c r="AF11" s="4"/>
     </row>
-    <row r="12" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="15"/>
-      <c r="B12" s="15"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="15"/>
-      <c r="E12" s="16" t="s">
+    <row r="12" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F12" s="17" t="s">
+      <c r="F12" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="G12" s="17" t="s">
+      <c r="G12" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H12" s="17" t="s">
+      <c r="H12" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I12" s="15"/>
-      <c r="J12" s="15"/>
-      <c r="K12" s="15"/>
-      <c r="L12" s="15"/>
-      <c r="M12" s="15"/>
-      <c r="N12" s="15"/>
-      <c r="O12" s="15"/>
-      <c r="P12" s="15"/>
-      <c r="Q12" s="15"/>
-      <c r="R12" s="15"/>
-      <c r="S12" s="15"/>
-      <c r="T12" s="15"/>
-      <c r="U12" s="15"/>
-      <c r="V12" s="15"/>
-      <c r="W12" s="15"/>
-      <c r="X12" s="15"/>
-      <c r="Y12" s="15"/>
-      <c r="Z12" s="15"/>
-      <c r="AA12" s="15"/>
-      <c r="AB12" s="15"/>
-      <c r="AC12" s="15"/>
-      <c r="AD12" s="15"/>
-      <c r="AE12" s="15"/>
-      <c r="AF12" s="15"/>
+      <c r="I12" s="9"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="M12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="9"/>
+      <c r="U12" s="9"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Y12" s="9"/>
+      <c r="Z12" s="9"/>
+      <c r="AA12" s="9"/>
+      <c r="AB12" s="9"/>
+      <c r="AC12" s="9"/>
+      <c r="AD12" s="9"/>
+      <c r="AE12" s="9"/>
+      <c r="AF12" s="9"/>
     </row>
     <row r="13" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
       <c r="D13" s="4"/>
-      <c r="E13" s="19" t="s">
+      <c r="E13" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F13" s="14" t="s">
+      <c r="F13" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="G13" s="14" t="s">
+      <c r="G13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H13" s="14" t="s">
+      <c r="H13" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I13" s="4"/>
@@ -1125,89 +1151,89 @@
       <c r="AE13" s="4"/>
       <c r="AF13" s="4"/>
     </row>
-    <row r="14" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="15"/>
-      <c r="B14" s="15"/>
-      <c r="C14" s="15"/>
-      <c r="D14" s="15"/>
-      <c r="E14" s="16" t="s">
+    <row r="14" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="9"/>
+      <c r="B14" s="9"/>
+      <c r="C14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F14" s="17" t="s">
+      <c r="F14" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="G14" s="17" t="s">
+      <c r="G14" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="17" t="s">
+      <c r="H14" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I14" s="15"/>
-      <c r="J14" s="15"/>
-      <c r="K14" s="15"/>
-      <c r="L14" s="15"/>
-      <c r="M14" s="15"/>
-      <c r="N14" s="15"/>
-      <c r="O14" s="15"/>
-      <c r="P14" s="15"/>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="15"/>
-      <c r="S14" s="15"/>
-      <c r="T14" s="15"/>
-      <c r="U14" s="15"/>
-      <c r="V14" s="15"/>
-      <c r="W14" s="15"/>
-      <c r="X14" s="15"/>
-      <c r="Y14" s="15"/>
-      <c r="Z14" s="15"/>
-      <c r="AA14" s="15"/>
-      <c r="AB14" s="15"/>
-      <c r="AC14" s="15"/>
-      <c r="AD14" s="15"/>
-      <c r="AE14" s="15"/>
-      <c r="AF14" s="15"/>
-    </row>
-    <row r="15" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="15"/>
-      <c r="B15" s="15"/>
-      <c r="C15" s="15"/>
-      <c r="D15" s="15"/>
-      <c r="E15" s="16" t="s">
+      <c r="I14" s="9"/>
+      <c r="J14" s="9"/>
+      <c r="K14" s="9"/>
+      <c r="L14" s="9"/>
+      <c r="M14" s="9"/>
+      <c r="N14" s="9"/>
+      <c r="O14" s="9"/>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="9"/>
+      <c r="U14" s="9"/>
+      <c r="V14" s="9"/>
+      <c r="W14" s="9"/>
+      <c r="X14" s="9"/>
+      <c r="Y14" s="9"/>
+      <c r="Z14" s="9"/>
+      <c r="AA14" s="9"/>
+      <c r="AB14" s="9"/>
+      <c r="AC14" s="9"/>
+      <c r="AD14" s="9"/>
+      <c r="AE14" s="9"/>
+      <c r="AF14" s="9"/>
+    </row>
+    <row r="15" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="9"/>
+      <c r="B15" s="9"/>
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="F15" s="17" t="s">
+      <c r="F15" s="11" t="s">
         <v>14</v>
       </c>
-      <c r="G15" s="17" t="s">
+      <c r="G15" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H15" s="17" t="s">
+      <c r="H15" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I15" s="15"/>
-      <c r="J15" s="15"/>
-      <c r="K15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="M15" s="15"/>
-      <c r="N15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="15"/>
-      <c r="Q15" s="15"/>
-      <c r="R15" s="15"/>
-      <c r="S15" s="15"/>
-      <c r="T15" s="15"/>
-      <c r="U15" s="15"/>
-      <c r="V15" s="15"/>
-      <c r="W15" s="15"/>
-      <c r="X15" s="15"/>
-      <c r="Y15" s="15"/>
-      <c r="Z15" s="15"/>
-      <c r="AA15" s="15"/>
-      <c r="AB15" s="15"/>
-      <c r="AC15" s="15"/>
-      <c r="AD15" s="15"/>
-      <c r="AE15" s="15"/>
-      <c r="AF15" s="15"/>
+      <c r="I15" s="9"/>
+      <c r="J15" s="9"/>
+      <c r="K15" s="9"/>
+      <c r="L15" s="9"/>
+      <c r="M15" s="9"/>
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="9"/>
+      <c r="U15" s="9"/>
+      <c r="V15" s="9"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="9"/>
+      <c r="Y15" s="9"/>
+      <c r="Z15" s="9"/>
+      <c r="AA15" s="9"/>
+      <c r="AB15" s="9"/>
+      <c r="AC15" s="9"/>
+      <c r="AD15" s="9"/>
+      <c r="AE15" s="9"/>
+      <c r="AF15" s="9"/>
     </row>
     <row r="16" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="4"/>
@@ -1256,16 +1282,16 @@
       <c r="B17" s="4"/>
       <c r="C17" s="4"/>
       <c r="D17" s="4"/>
-      <c r="E17" s="19" t="s">
+      <c r="E17" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F17" s="14" t="s">
+      <c r="F17" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="G17" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H17" s="14" t="s">
+      <c r="G17" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H17" s="8" t="s">
         <v>13</v>
       </c>
       <c r="I17" s="4"/>
@@ -1293,105 +1319,105 @@
       <c r="AE17" s="4"/>
       <c r="AF17" s="4"/>
     </row>
-    <row r="18" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="15"/>
-      <c r="B18" s="15"/>
-      <c r="C18" s="15"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="16" t="s">
+    <row r="18" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="9"/>
+      <c r="B18" s="9"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="17" t="s">
+      <c r="F18" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="G18" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H18" s="17" t="s">
+      <c r="G18" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H18" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15"/>
-      <c r="M18" s="15"/>
-      <c r="N18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15"/>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="15"/>
-      <c r="S18" s="15"/>
-      <c r="T18" s="15"/>
-      <c r="U18" s="15"/>
-      <c r="V18" s="15"/>
-      <c r="W18" s="15"/>
-      <c r="X18" s="15"/>
-      <c r="Y18" s="15"/>
-      <c r="Z18" s="15"/>
-      <c r="AA18" s="15"/>
-      <c r="AB18" s="15"/>
-      <c r="AC18" s="15"/>
-      <c r="AD18" s="15"/>
-      <c r="AE18" s="15"/>
-      <c r="AF18" s="15"/>
-    </row>
-    <row r="19" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15"/>
-      <c r="B19" s="15"/>
-      <c r="C19" s="15"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="16" t="s">
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
+      <c r="T18" s="9"/>
+      <c r="U18" s="9"/>
+      <c r="V18" s="9"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="9"/>
+      <c r="Y18" s="9"/>
+      <c r="Z18" s="9"/>
+      <c r="AA18" s="9"/>
+      <c r="AB18" s="9"/>
+      <c r="AC18" s="9"/>
+      <c r="AD18" s="9"/>
+      <c r="AE18" s="9"/>
+      <c r="AF18" s="9"/>
+    </row>
+    <row r="19" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="B19" s="9"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="17" t="s">
+      <c r="F19" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="G19" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H19" s="17" t="s">
+      <c r="G19" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H19" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15"/>
-      <c r="M19" s="15"/>
-      <c r="N19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="15"/>
-      <c r="S19" s="15"/>
-      <c r="T19" s="15"/>
-      <c r="U19" s="15"/>
-      <c r="V19" s="15"/>
-      <c r="W19" s="15"/>
-      <c r="X19" s="15"/>
-      <c r="Y19" s="15"/>
-      <c r="Z19" s="15"/>
-      <c r="AA19" s="15"/>
-      <c r="AB19" s="15"/>
-      <c r="AC19" s="15"/>
-      <c r="AD19" s="15"/>
-      <c r="AE19" s="15"/>
-      <c r="AF19" s="15"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="9"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="9"/>
+      <c r="M19" s="9"/>
+      <c r="N19" s="9"/>
+      <c r="O19" s="9"/>
+      <c r="P19" s="9"/>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
+      <c r="T19" s="9"/>
+      <c r="U19" s="9"/>
+      <c r="V19" s="9"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="9"/>
+      <c r="Y19" s="9"/>
+      <c r="Z19" s="9"/>
+      <c r="AA19" s="9"/>
+      <c r="AB19" s="9"/>
+      <c r="AC19" s="9"/>
+      <c r="AD19" s="9"/>
+      <c r="AE19" s="9"/>
+      <c r="AF19" s="9"/>
     </row>
     <row r="20" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="4"/>
       <c r="B20" s="4"/>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="19" t="s">
+      <c r="E20" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F20" s="14" t="s">
+      <c r="F20" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="G20" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H20" s="14" t="s">
+      <c r="G20" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H20" s="8" t="s">
         <v>13</v>
       </c>
       <c r="I20" s="4"/>
@@ -1419,105 +1445,105 @@
       <c r="AE20" s="4"/>
       <c r="AF20" s="4"/>
     </row>
-    <row r="21" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="15"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="16" t="s">
+    <row r="21" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="9"/>
+      <c r="B21" s="9"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F21" s="17" t="s">
+      <c r="F21" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="G21" s="17" t="s">
+      <c r="G21" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H21" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="9"/>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
+      <c r="T21" s="9"/>
+      <c r="U21" s="9"/>
+      <c r="V21" s="9"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="9"/>
+      <c r="Y21" s="9"/>
+      <c r="Z21" s="9"/>
+      <c r="AA21" s="9"/>
+      <c r="AB21" s="9"/>
+      <c r="AC21" s="9"/>
+      <c r="AD21" s="9"/>
+      <c r="AE21" s="9"/>
+      <c r="AF21" s="9"/>
+    </row>
+    <row r="22" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="9"/>
+      <c r="B22" s="9"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F22" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="G22" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="H21" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="M21" s="15"/>
-      <c r="N21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15"/>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="15"/>
-      <c r="S21" s="15"/>
-      <c r="T21" s="15"/>
-      <c r="U21" s="15"/>
-      <c r="V21" s="15"/>
-      <c r="W21" s="15"/>
-      <c r="X21" s="15"/>
-      <c r="Y21" s="15"/>
-      <c r="Z21" s="15"/>
-      <c r="AA21" s="15"/>
-      <c r="AB21" s="15"/>
-      <c r="AC21" s="15"/>
-      <c r="AD21" s="15"/>
-      <c r="AE21" s="15"/>
-      <c r="AF21" s="15"/>
-    </row>
-    <row r="22" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="15"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="16" t="s">
-        <v>29</v>
-      </c>
-      <c r="F22" s="17" t="s">
-        <v>23</v>
-      </c>
-      <c r="G22" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="H22" s="17" t="s">
+      <c r="H22" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="M22" s="15"/>
-      <c r="N22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15"/>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="15"/>
-      <c r="S22" s="15"/>
-      <c r="T22" s="15"/>
-      <c r="U22" s="15"/>
-      <c r="V22" s="15"/>
-      <c r="W22" s="15"/>
-      <c r="X22" s="15"/>
-      <c r="Y22" s="15"/>
-      <c r="Z22" s="15"/>
-      <c r="AA22" s="15"/>
-      <c r="AB22" s="15"/>
-      <c r="AC22" s="15"/>
-      <c r="AD22" s="15"/>
-      <c r="AE22" s="15"/>
-      <c r="AF22" s="15"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
+      <c r="T22" s="9"/>
+      <c r="U22" s="9"/>
+      <c r="V22" s="9"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="9"/>
+      <c r="Y22" s="9"/>
+      <c r="Z22" s="9"/>
+      <c r="AA22" s="9"/>
+      <c r="AB22" s="9"/>
+      <c r="AC22" s="9"/>
+      <c r="AD22" s="9"/>
+      <c r="AE22" s="9"/>
+      <c r="AF22" s="9"/>
     </row>
     <row r="23" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="4"/>
       <c r="B23" s="4"/>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="14" t="s">
+      <c r="F23" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="G23" s="14" t="s">
+      <c r="G23" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="14" t="s">
+      <c r="H23" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I23" s="4"/>
@@ -1545,105 +1571,105 @@
       <c r="AE23" s="4"/>
       <c r="AF23" s="4"/>
     </row>
-    <row r="24" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="15"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="16" t="s">
+    <row r="24" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="B24" s="9"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F24" s="17" t="s">
-        <v>70</v>
-      </c>
-      <c r="G24" s="17" t="s">
+      <c r="F24" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="G24" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H24" s="17" t="s">
+      <c r="H24" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I24" s="15"/>
-      <c r="J24" s="15"/>
-      <c r="K24" s="15"/>
-      <c r="L24" s="15"/>
-      <c r="M24" s="15"/>
-      <c r="N24" s="15"/>
-      <c r="O24" s="15"/>
-      <c r="P24" s="15"/>
-      <c r="Q24" s="15"/>
-      <c r="R24" s="15"/>
-      <c r="S24" s="15"/>
-      <c r="T24" s="15"/>
-      <c r="U24" s="15"/>
-      <c r="V24" s="15"/>
-      <c r="W24" s="15"/>
-      <c r="X24" s="15"/>
-      <c r="Y24" s="15"/>
-      <c r="Z24" s="15"/>
-      <c r="AA24" s="15"/>
-      <c r="AB24" s="15"/>
-      <c r="AC24" s="15"/>
-      <c r="AD24" s="15"/>
-      <c r="AE24" s="15"/>
-      <c r="AF24" s="15"/>
-    </row>
-    <row r="25" spans="1:32" s="18" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="15"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="16" t="s">
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="9"/>
+      <c r="U24" s="9"/>
+      <c r="V24" s="9"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="9"/>
+      <c r="Y24" s="9"/>
+      <c r="Z24" s="9"/>
+      <c r="AA24" s="9"/>
+      <c r="AB24" s="9"/>
+      <c r="AC24" s="9"/>
+      <c r="AD24" s="9"/>
+      <c r="AE24" s="9"/>
+      <c r="AF24" s="9"/>
+    </row>
+    <row r="25" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="B25" s="9"/>
+      <c r="C25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F25" s="17" t="s">
+      <c r="F25" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="G25" s="17" t="s">
+      <c r="G25" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H25" s="17" t="s">
+      <c r="H25" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I25" s="15"/>
-      <c r="J25" s="15"/>
-      <c r="K25" s="15"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="15"/>
-      <c r="N25" s="15"/>
-      <c r="O25" s="15"/>
-      <c r="P25" s="15"/>
-      <c r="Q25" s="15"/>
-      <c r="R25" s="15"/>
-      <c r="S25" s="15"/>
-      <c r="T25" s="15"/>
-      <c r="U25" s="15"/>
-      <c r="V25" s="15"/>
-      <c r="W25" s="15"/>
-      <c r="X25" s="15"/>
-      <c r="Y25" s="15"/>
-      <c r="Z25" s="15"/>
-      <c r="AA25" s="15"/>
-      <c r="AB25" s="15"/>
-      <c r="AC25" s="15"/>
-      <c r="AD25" s="15"/>
-      <c r="AE25" s="15"/>
-      <c r="AF25" s="15"/>
+      <c r="I25" s="9"/>
+      <c r="J25" s="9"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="9"/>
+      <c r="M25" s="9"/>
+      <c r="N25" s="9"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="9"/>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
+      <c r="T25" s="9"/>
+      <c r="U25" s="9"/>
+      <c r="V25" s="9"/>
+      <c r="W25" s="9"/>
+      <c r="X25" s="9"/>
+      <c r="Y25" s="9"/>
+      <c r="Z25" s="9"/>
+      <c r="AA25" s="9"/>
+      <c r="AB25" s="9"/>
+      <c r="AC25" s="9"/>
+      <c r="AD25" s="9"/>
+      <c r="AE25" s="9"/>
+      <c r="AF25" s="9"/>
     </row>
     <row r="26" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="4"/>
       <c r="B26" s="4"/>
       <c r="C26" s="4"/>
       <c r="D26" s="4"/>
-      <c r="E26" s="19" t="s">
+      <c r="E26" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F26" s="14" t="s">
+      <c r="F26" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="G26" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H26" s="14" t="s">
+      <c r="G26" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H26" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I26" s="4"/>
@@ -1671,257 +1697,257 @@
       <c r="AE26" s="4"/>
       <c r="AF26" s="4"/>
     </row>
-    <row r="27" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="15"/>
-      <c r="B27" s="15"/>
-      <c r="C27" s="15"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="16" t="s">
+    <row r="27" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="9"/>
+      <c r="B27" s="9"/>
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="G27" s="17" t="s">
+      <c r="G27" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H27" s="17" t="s">
+      <c r="H27" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I27" s="15"/>
-      <c r="J27" s="15"/>
-      <c r="K27" s="15"/>
-      <c r="L27" s="15"/>
-      <c r="M27" s="15"/>
-      <c r="N27" s="15"/>
-      <c r="O27" s="15"/>
-      <c r="P27" s="15"/>
-      <c r="Q27" s="15"/>
-      <c r="R27" s="15"/>
-      <c r="S27" s="15"/>
-      <c r="T27" s="15"/>
-      <c r="U27" s="15"/>
-      <c r="V27" s="15"/>
-      <c r="W27" s="15"/>
-      <c r="X27" s="15"/>
-      <c r="Y27" s="15"/>
-      <c r="Z27" s="15"/>
-      <c r="AA27" s="15"/>
-      <c r="AB27" s="15"/>
-      <c r="AC27" s="15"/>
-      <c r="AD27" s="15"/>
-      <c r="AE27" s="15"/>
-      <c r="AF27" s="15"/>
-    </row>
-    <row r="28" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="15"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="16" t="s">
+      <c r="I27" s="9"/>
+      <c r="J27" s="9"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="9"/>
+      <c r="M27" s="9"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
+      <c r="T27" s="9"/>
+      <c r="U27" s="9"/>
+      <c r="V27" s="9"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="9"/>
+      <c r="Y27" s="9"/>
+      <c r="Z27" s="9"/>
+      <c r="AA27" s="9"/>
+      <c r="AB27" s="9"/>
+      <c r="AC27" s="9"/>
+      <c r="AD27" s="9"/>
+      <c r="AE27" s="9"/>
+      <c r="AF27" s="9"/>
+    </row>
+    <row r="28" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9"/>
+      <c r="B28" s="9"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F28" s="17" t="s">
+      <c r="F28" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="G28" s="17" t="s">
+      <c r="G28" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H28" s="17" t="s">
+      <c r="H28" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I28" s="15"/>
-      <c r="J28" s="15"/>
-      <c r="K28" s="15"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="15"/>
-      <c r="N28" s="15"/>
-      <c r="O28" s="15"/>
-      <c r="P28" s="15"/>
-      <c r="Q28" s="15"/>
-      <c r="R28" s="15"/>
-      <c r="S28" s="15"/>
-      <c r="T28" s="15"/>
-      <c r="U28" s="15"/>
-      <c r="V28" s="15"/>
-      <c r="W28" s="15"/>
-      <c r="X28" s="15"/>
-      <c r="Y28" s="15"/>
-      <c r="Z28" s="15"/>
-      <c r="AA28" s="15"/>
-      <c r="AB28" s="15"/>
-      <c r="AC28" s="15"/>
-      <c r="AD28" s="15"/>
-      <c r="AE28" s="15"/>
-      <c r="AF28" s="15"/>
-    </row>
-    <row r="29" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="15"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="19" t="s">
+      <c r="I28" s="9"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="9"/>
+      <c r="M28" s="9"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
+      <c r="T28" s="9"/>
+      <c r="U28" s="9"/>
+      <c r="V28" s="9"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="9"/>
+      <c r="Y28" s="9"/>
+      <c r="Z28" s="9"/>
+      <c r="AA28" s="9"/>
+      <c r="AB28" s="9"/>
+      <c r="AC28" s="9"/>
+      <c r="AD28" s="9"/>
+      <c r="AE28" s="9"/>
+      <c r="AF28" s="9"/>
+    </row>
+    <row r="29" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="9"/>
+      <c r="B29" s="9"/>
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="F29" s="14" t="s">
+      <c r="F29" s="8" t="s">
         <v>33</v>
       </c>
-      <c r="G29" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H29" s="14" t="s">
+      <c r="G29" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H29" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="I29" s="15"/>
-      <c r="J29" s="15"/>
-      <c r="K29" s="15"/>
-      <c r="L29" s="15"/>
-      <c r="M29" s="15"/>
-      <c r="N29" s="15"/>
-      <c r="O29" s="15"/>
-      <c r="P29" s="15"/>
-      <c r="Q29" s="15"/>
-      <c r="R29" s="15"/>
-      <c r="S29" s="15"/>
-      <c r="T29" s="15"/>
-      <c r="U29" s="15"/>
-      <c r="V29" s="15"/>
-      <c r="W29" s="15"/>
-      <c r="X29" s="15"/>
-      <c r="Y29" s="15"/>
-      <c r="Z29" s="15"/>
-      <c r="AA29" s="15"/>
-      <c r="AB29" s="15"/>
-      <c r="AC29" s="15"/>
-      <c r="AD29" s="15"/>
-      <c r="AE29" s="15"/>
-      <c r="AF29" s="15"/>
-    </row>
-    <row r="30" spans="1:32" s="18" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="15"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="16" t="s">
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
+      <c r="T29" s="9"/>
+      <c r="U29" s="9"/>
+      <c r="V29" s="9"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="9"/>
+      <c r="Y29" s="9"/>
+      <c r="Z29" s="9"/>
+      <c r="AA29" s="9"/>
+      <c r="AB29" s="9"/>
+      <c r="AC29" s="9"/>
+      <c r="AD29" s="9"/>
+      <c r="AE29" s="9"/>
+      <c r="AF29" s="9"/>
+    </row>
+    <row r="30" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="9"/>
+      <c r="B30" s="9"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F30" s="17" t="s">
+      <c r="F30" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="G30" s="17" t="s">
+      <c r="G30" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H30" s="17" t="s">
+      <c r="H30" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I30" s="15"/>
-      <c r="J30" s="15"/>
-      <c r="K30" s="15"/>
-      <c r="L30" s="15"/>
-      <c r="M30" s="15"/>
-      <c r="N30" s="15"/>
-      <c r="O30" s="15"/>
-      <c r="P30" s="15"/>
-      <c r="Q30" s="15"/>
-      <c r="R30" s="15"/>
-      <c r="S30" s="15"/>
-      <c r="T30" s="15"/>
-      <c r="U30" s="15"/>
-      <c r="V30" s="15"/>
-      <c r="W30" s="15"/>
-      <c r="X30" s="15"/>
-      <c r="Y30" s="15"/>
-      <c r="Z30" s="15"/>
-      <c r="AA30" s="15"/>
-      <c r="AB30" s="15"/>
-      <c r="AC30" s="15"/>
-      <c r="AD30" s="15"/>
-      <c r="AE30" s="15"/>
-      <c r="AF30" s="15"/>
-    </row>
-    <row r="31" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="15"/>
-      <c r="D31" s="15"/>
-      <c r="E31" s="16" t="s">
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="9"/>
+      <c r="N30" s="9"/>
+      <c r="O30" s="9"/>
+      <c r="P30" s="9"/>
+      <c r="Q30" s="9"/>
+      <c r="R30" s="9"/>
+      <c r="S30" s="9"/>
+      <c r="T30" s="9"/>
+      <c r="U30" s="9"/>
+      <c r="V30" s="9"/>
+      <c r="W30" s="9"/>
+      <c r="X30" s="9"/>
+      <c r="Y30" s="9"/>
+      <c r="Z30" s="9"/>
+      <c r="AA30" s="9"/>
+      <c r="AB30" s="9"/>
+      <c r="AC30" s="9"/>
+      <c r="AD30" s="9"/>
+      <c r="AE30" s="9"/>
+      <c r="AF30" s="9"/>
+    </row>
+    <row r="31" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9"/>
+      <c r="B31" s="9"/>
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F31" s="17" t="s">
+      <c r="F31" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="G31" s="17" t="s">
+      <c r="G31" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="H31" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I31" s="15"/>
-      <c r="J31" s="15"/>
-      <c r="K31" s="15"/>
-      <c r="L31" s="15"/>
-      <c r="M31" s="15"/>
-      <c r="N31" s="15"/>
-      <c r="O31" s="15"/>
-      <c r="P31" s="15"/>
-      <c r="Q31" s="15"/>
-      <c r="R31" s="15"/>
-      <c r="S31" s="15"/>
-      <c r="T31" s="15"/>
-      <c r="U31" s="15"/>
-      <c r="V31" s="15"/>
-      <c r="W31" s="15"/>
-      <c r="X31" s="15"/>
-      <c r="Y31" s="15"/>
-      <c r="Z31" s="15"/>
-      <c r="AA31" s="15"/>
-      <c r="AB31" s="15"/>
-      <c r="AC31" s="15"/>
-      <c r="AD31" s="15"/>
-      <c r="AE31" s="15"/>
-      <c r="AF31" s="15"/>
-    </row>
-    <row r="32" spans="1:32" s="18" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15"/>
-      <c r="B32" s="15"/>
-      <c r="C32" s="15"/>
-      <c r="D32" s="15"/>
-      <c r="E32" s="16" t="s">
+      <c r="I31" s="9"/>
+      <c r="J31" s="9"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="9"/>
+      <c r="O31" s="9"/>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
+      <c r="T31" s="9"/>
+      <c r="U31" s="9"/>
+      <c r="V31" s="9"/>
+      <c r="W31" s="9"/>
+      <c r="X31" s="9"/>
+      <c r="Y31" s="9"/>
+      <c r="Z31" s="9"/>
+      <c r="AA31" s="9"/>
+      <c r="AB31" s="9"/>
+      <c r="AC31" s="9"/>
+      <c r="AD31" s="9"/>
+      <c r="AE31" s="9"/>
+      <c r="AF31" s="9"/>
+    </row>
+    <row r="32" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="9"/>
+      <c r="B32" s="9"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="F32" s="17" t="s">
+      <c r="F32" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="G32" s="17" t="s">
+      <c r="G32" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H32" s="17" t="s">
+      <c r="H32" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I32" s="15"/>
-      <c r="J32" s="15"/>
-      <c r="K32" s="15"/>
-      <c r="L32" s="15"/>
-      <c r="M32" s="15"/>
-      <c r="N32" s="15"/>
-      <c r="O32" s="15"/>
-      <c r="P32" s="15"/>
-      <c r="Q32" s="15"/>
-      <c r="R32" s="15"/>
-      <c r="S32" s="15"/>
-      <c r="T32" s="15"/>
-      <c r="U32" s="15"/>
-      <c r="V32" s="15"/>
-      <c r="W32" s="15"/>
-      <c r="X32" s="15"/>
-      <c r="Y32" s="15"/>
-      <c r="Z32" s="15"/>
-      <c r="AA32" s="15"/>
-      <c r="AB32" s="15"/>
-      <c r="AC32" s="15"/>
-      <c r="AD32" s="15"/>
-      <c r="AE32" s="15"/>
-      <c r="AF32" s="15"/>
+      <c r="I32" s="9"/>
+      <c r="J32" s="9"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="9"/>
+      <c r="M32" s="9"/>
+      <c r="N32" s="9"/>
+      <c r="O32" s="9"/>
+      <c r="P32" s="9"/>
+      <c r="Q32" s="9"/>
+      <c r="R32" s="9"/>
+      <c r="S32" s="9"/>
+      <c r="T32" s="9"/>
+      <c r="U32" s="9"/>
+      <c r="V32" s="9"/>
+      <c r="W32" s="9"/>
+      <c r="X32" s="9"/>
+      <c r="Y32" s="9"/>
+      <c r="Z32" s="9"/>
+      <c r="AA32" s="9"/>
+      <c r="AB32" s="9"/>
+      <c r="AC32" s="9"/>
+      <c r="AD32" s="9"/>
+      <c r="AE32" s="9"/>
+      <c r="AF32" s="9"/>
     </row>
     <row r="33" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
@@ -1970,16 +1996,16 @@
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
-      <c r="E34" s="19" t="s">
+      <c r="E34" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F34" s="14" t="s">
+      <c r="F34" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="G34" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H34" s="14" t="s">
+      <c r="G34" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H34" s="8" t="s">
         <v>13</v>
       </c>
       <c r="I34" s="4"/>
@@ -2007,105 +2033,105 @@
       <c r="AE34" s="4"/>
       <c r="AF34" s="4"/>
     </row>
-    <row r="35" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A35" s="15"/>
-      <c r="B35" s="15"/>
-      <c r="C35" s="15"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="16" t="s">
+    <row r="35" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="9"/>
+      <c r="C35" s="9"/>
+      <c r="D35" s="9"/>
+      <c r="E35" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F35" s="17" t="s">
+      <c r="F35" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="G35" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H35" s="17" t="s">
+      <c r="G35" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H35" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I35" s="15"/>
-      <c r="J35" s="15"/>
-      <c r="K35" s="15"/>
-      <c r="L35" s="15"/>
-      <c r="M35" s="15"/>
-      <c r="N35" s="15"/>
-      <c r="O35" s="15"/>
-      <c r="P35" s="15"/>
-      <c r="Q35" s="15"/>
-      <c r="R35" s="15"/>
-      <c r="S35" s="15"/>
-      <c r="T35" s="15"/>
-      <c r="U35" s="15"/>
-      <c r="V35" s="15"/>
-      <c r="W35" s="15"/>
-      <c r="X35" s="15"/>
-      <c r="Y35" s="15"/>
-      <c r="Z35" s="15"/>
-      <c r="AA35" s="15"/>
-      <c r="AB35" s="15"/>
-      <c r="AC35" s="15"/>
-      <c r="AD35" s="15"/>
-      <c r="AE35" s="15"/>
-      <c r="AF35" s="15"/>
-    </row>
-    <row r="36" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A36" s="15"/>
-      <c r="B36" s="15"/>
-      <c r="C36" s="15"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="16" t="s">
+      <c r="I35" s="9"/>
+      <c r="J35" s="9"/>
+      <c r="K35" s="9"/>
+      <c r="L35" s="9"/>
+      <c r="M35" s="9"/>
+      <c r="N35" s="9"/>
+      <c r="O35" s="9"/>
+      <c r="P35" s="9"/>
+      <c r="Q35" s="9"/>
+      <c r="R35" s="9"/>
+      <c r="S35" s="9"/>
+      <c r="T35" s="9"/>
+      <c r="U35" s="9"/>
+      <c r="V35" s="9"/>
+      <c r="W35" s="9"/>
+      <c r="X35" s="9"/>
+      <c r="Y35" s="9"/>
+      <c r="Z35" s="9"/>
+      <c r="AA35" s="9"/>
+      <c r="AB35" s="9"/>
+      <c r="AC35" s="9"/>
+      <c r="AD35" s="9"/>
+      <c r="AE35" s="9"/>
+      <c r="AF35" s="9"/>
+    </row>
+    <row r="36" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="9"/>
+      <c r="B36" s="9"/>
+      <c r="C36" s="9"/>
+      <c r="D36" s="9"/>
+      <c r="E36" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F36" s="17" t="s">
+      <c r="F36" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="G36" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H36" s="17" t="s">
+      <c r="G36" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H36" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I36" s="15"/>
-      <c r="J36" s="15"/>
-      <c r="K36" s="15"/>
-      <c r="L36" s="15"/>
-      <c r="M36" s="15"/>
-      <c r="N36" s="15"/>
-      <c r="O36" s="15"/>
-      <c r="P36" s="15"/>
-      <c r="Q36" s="15"/>
-      <c r="R36" s="15"/>
-      <c r="S36" s="15"/>
-      <c r="T36" s="15"/>
-      <c r="U36" s="15"/>
-      <c r="V36" s="15"/>
-      <c r="W36" s="15"/>
-      <c r="X36" s="15"/>
-      <c r="Y36" s="15"/>
-      <c r="Z36" s="15"/>
-      <c r="AA36" s="15"/>
-      <c r="AB36" s="15"/>
-      <c r="AC36" s="15"/>
-      <c r="AD36" s="15"/>
-      <c r="AE36" s="15"/>
-      <c r="AF36" s="15"/>
+      <c r="I36" s="9"/>
+      <c r="J36" s="9"/>
+      <c r="K36" s="9"/>
+      <c r="L36" s="9"/>
+      <c r="M36" s="9"/>
+      <c r="N36" s="9"/>
+      <c r="O36" s="9"/>
+      <c r="P36" s="9"/>
+      <c r="Q36" s="9"/>
+      <c r="R36" s="9"/>
+      <c r="S36" s="9"/>
+      <c r="T36" s="9"/>
+      <c r="U36" s="9"/>
+      <c r="V36" s="9"/>
+      <c r="W36" s="9"/>
+      <c r="X36" s="9"/>
+      <c r="Y36" s="9"/>
+      <c r="Z36" s="9"/>
+      <c r="AA36" s="9"/>
+      <c r="AB36" s="9"/>
+      <c r="AC36" s="9"/>
+      <c r="AD36" s="9"/>
+      <c r="AE36" s="9"/>
+      <c r="AF36" s="9"/>
     </row>
     <row r="37" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
-      <c r="E37" s="19" t="s">
+      <c r="E37" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F37" s="14" t="s">
+      <c r="F37" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="G37" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H37" s="14" t="s">
+      <c r="G37" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H37" s="8" t="s">
         <v>13</v>
       </c>
       <c r="I37" s="4"/>
@@ -2133,63 +2159,63 @@
       <c r="AE37" s="4"/>
       <c r="AF37" s="4"/>
     </row>
-    <row r="38" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A38" s="15"/>
-      <c r="B38" s="15"/>
-      <c r="C38" s="15"/>
-      <c r="D38" s="15"/>
-      <c r="E38" s="16" t="s">
+    <row r="38" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="9"/>
+      <c r="B38" s="9"/>
+      <c r="C38" s="9"/>
+      <c r="D38" s="9"/>
+      <c r="E38" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F38" s="17" t="s">
+      <c r="F38" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="G38" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H38" s="17" t="s">
+      <c r="G38" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H38" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I38" s="15"/>
-      <c r="J38" s="15"/>
-      <c r="K38" s="15"/>
-      <c r="L38" s="15"/>
-      <c r="M38" s="15"/>
-      <c r="N38" s="15"/>
-      <c r="O38" s="15"/>
-      <c r="P38" s="15"/>
-      <c r="Q38" s="15"/>
-      <c r="R38" s="15"/>
-      <c r="S38" s="15"/>
-      <c r="T38" s="15"/>
-      <c r="U38" s="15"/>
-      <c r="V38" s="15"/>
-      <c r="W38" s="15"/>
-      <c r="X38" s="15"/>
-      <c r="Y38" s="15"/>
-      <c r="Z38" s="15"/>
-      <c r="AA38" s="15"/>
-      <c r="AB38" s="15"/>
-      <c r="AC38" s="15"/>
-      <c r="AD38" s="15"/>
-      <c r="AE38" s="15"/>
-      <c r="AF38" s="15"/>
+      <c r="I38" s="9"/>
+      <c r="J38" s="9"/>
+      <c r="K38" s="9"/>
+      <c r="L38" s="9"/>
+      <c r="M38" s="9"/>
+      <c r="N38" s="9"/>
+      <c r="O38" s="9"/>
+      <c r="P38" s="9"/>
+      <c r="Q38" s="9"/>
+      <c r="R38" s="9"/>
+      <c r="S38" s="9"/>
+      <c r="T38" s="9"/>
+      <c r="U38" s="9"/>
+      <c r="V38" s="9"/>
+      <c r="W38" s="9"/>
+      <c r="X38" s="9"/>
+      <c r="Y38" s="9"/>
+      <c r="Z38" s="9"/>
+      <c r="AA38" s="9"/>
+      <c r="AB38" s="9"/>
+      <c r="AC38" s="9"/>
+      <c r="AD38" s="9"/>
+      <c r="AE38" s="9"/>
+      <c r="AF38" s="9"/>
     </row>
     <row r="39" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
-      <c r="E39" s="19" t="s">
+      <c r="E39" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F39" s="14" t="s">
+      <c r="F39" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="G39" s="14" t="s">
+      <c r="G39" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H39" s="14" t="s">
+      <c r="H39" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I39" s="4"/>
@@ -2217,105 +2243,105 @@
       <c r="AE39" s="4"/>
       <c r="AF39" s="4"/>
     </row>
-    <row r="40" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A40" s="15"/>
-      <c r="B40" s="15"/>
-      <c r="C40" s="15"/>
-      <c r="D40" s="15"/>
-      <c r="E40" s="16" t="s">
+    <row r="40" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="9"/>
+      <c r="B40" s="9"/>
+      <c r="C40" s="9"/>
+      <c r="D40" s="9"/>
+      <c r="E40" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F40" s="17" t="s">
+      <c r="F40" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="G40" s="17" t="s">
+      <c r="G40" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H40" s="17" t="s">
+      <c r="H40" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I40" s="15"/>
-      <c r="J40" s="15"/>
-      <c r="K40" s="15"/>
-      <c r="L40" s="15"/>
-      <c r="M40" s="15"/>
-      <c r="N40" s="15"/>
-      <c r="O40" s="15"/>
-      <c r="P40" s="15"/>
-      <c r="Q40" s="15"/>
-      <c r="R40" s="15"/>
-      <c r="S40" s="15"/>
-      <c r="T40" s="15"/>
-      <c r="U40" s="15"/>
-      <c r="V40" s="15"/>
-      <c r="W40" s="15"/>
-      <c r="X40" s="15"/>
-      <c r="Y40" s="15"/>
-      <c r="Z40" s="15"/>
-      <c r="AA40" s="15"/>
-      <c r="AB40" s="15"/>
-      <c r="AC40" s="15"/>
-      <c r="AD40" s="15"/>
-      <c r="AE40" s="15"/>
-      <c r="AF40" s="15"/>
-    </row>
-    <row r="41" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A41" s="15"/>
-      <c r="B41" s="15"/>
-      <c r="C41" s="15"/>
-      <c r="D41" s="15"/>
-      <c r="E41" s="16" t="s">
+      <c r="I40" s="9"/>
+      <c r="J40" s="9"/>
+      <c r="K40" s="9"/>
+      <c r="L40" s="9"/>
+      <c r="M40" s="9"/>
+      <c r="N40" s="9"/>
+      <c r="O40" s="9"/>
+      <c r="P40" s="9"/>
+      <c r="Q40" s="9"/>
+      <c r="R40" s="9"/>
+      <c r="S40" s="9"/>
+      <c r="T40" s="9"/>
+      <c r="U40" s="9"/>
+      <c r="V40" s="9"/>
+      <c r="W40" s="9"/>
+      <c r="X40" s="9"/>
+      <c r="Y40" s="9"/>
+      <c r="Z40" s="9"/>
+      <c r="AA40" s="9"/>
+      <c r="AB40" s="9"/>
+      <c r="AC40" s="9"/>
+      <c r="AD40" s="9"/>
+      <c r="AE40" s="9"/>
+      <c r="AF40" s="9"/>
+    </row>
+    <row r="41" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A41" s="9"/>
+      <c r="B41" s="9"/>
+      <c r="C41" s="9"/>
+      <c r="D41" s="9"/>
+      <c r="E41" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F41" s="17" t="s">
+      <c r="F41" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="G41" s="17" t="s">
+      <c r="G41" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H41" s="17" t="s">
+      <c r="H41" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I41" s="15"/>
-      <c r="J41" s="15"/>
-      <c r="K41" s="15"/>
-      <c r="L41" s="15"/>
-      <c r="M41" s="15"/>
-      <c r="N41" s="15"/>
-      <c r="O41" s="15"/>
-      <c r="P41" s="15"/>
-      <c r="Q41" s="15"/>
-      <c r="R41" s="15"/>
-      <c r="S41" s="15"/>
-      <c r="T41" s="15"/>
-      <c r="U41" s="15"/>
-      <c r="V41" s="15"/>
-      <c r="W41" s="15"/>
-      <c r="X41" s="15"/>
-      <c r="Y41" s="15"/>
-      <c r="Z41" s="15"/>
-      <c r="AA41" s="15"/>
-      <c r="AB41" s="15"/>
-      <c r="AC41" s="15"/>
-      <c r="AD41" s="15"/>
-      <c r="AE41" s="15"/>
-      <c r="AF41" s="15"/>
+      <c r="I41" s="9"/>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="9"/>
+      <c r="U41" s="9"/>
+      <c r="V41" s="9"/>
+      <c r="W41" s="9"/>
+      <c r="X41" s="9"/>
+      <c r="Y41" s="9"/>
+      <c r="Z41" s="9"/>
+      <c r="AA41" s="9"/>
+      <c r="AB41" s="9"/>
+      <c r="AC41" s="9"/>
+      <c r="AD41" s="9"/>
+      <c r="AE41" s="9"/>
+      <c r="AF41" s="9"/>
     </row>
     <row r="42" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="19" t="s">
+      <c r="E42" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F42" s="14" t="s">
+      <c r="F42" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="G42" s="14" t="s">
+      <c r="G42" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H42" s="14" t="s">
+      <c r="H42" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I42" s="4"/>
@@ -2343,105 +2369,105 @@
       <c r="AE42" s="4"/>
       <c r="AF42" s="4"/>
     </row>
-    <row r="43" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="15"/>
-      <c r="B43" s="15"/>
-      <c r="C43" s="15"/>
-      <c r="D43" s="15"/>
-      <c r="E43" s="16" t="s">
+    <row r="43" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F43" s="17" t="s">
+      <c r="F43" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="G43" s="17" t="s">
+      <c r="G43" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H43" s="17" t="s">
+      <c r="H43" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I43" s="15"/>
-      <c r="J43" s="15"/>
-      <c r="K43" s="15"/>
-      <c r="L43" s="15"/>
-      <c r="M43" s="15"/>
-      <c r="N43" s="15"/>
-      <c r="O43" s="15"/>
-      <c r="P43" s="15"/>
-      <c r="Q43" s="15"/>
-      <c r="R43" s="15"/>
-      <c r="S43" s="15"/>
-      <c r="T43" s="15"/>
-      <c r="U43" s="15"/>
-      <c r="V43" s="15"/>
-      <c r="W43" s="15"/>
-      <c r="X43" s="15"/>
-      <c r="Y43" s="15"/>
-      <c r="Z43" s="15"/>
-      <c r="AA43" s="15"/>
-      <c r="AB43" s="15"/>
-      <c r="AC43" s="15"/>
-      <c r="AD43" s="15"/>
-      <c r="AE43" s="15"/>
-      <c r="AF43" s="15"/>
-    </row>
-    <row r="44" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="15"/>
-      <c r="B44" s="15"/>
-      <c r="C44" s="15"/>
-      <c r="D44" s="15"/>
-      <c r="E44" s="16" t="s">
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="9"/>
+      <c r="V43" s="9"/>
+      <c r="W43" s="9"/>
+      <c r="X43" s="9"/>
+      <c r="Y43" s="9"/>
+      <c r="Z43" s="9"/>
+      <c r="AA43" s="9"/>
+      <c r="AB43" s="9"/>
+      <c r="AC43" s="9"/>
+      <c r="AD43" s="9"/>
+      <c r="AE43" s="9"/>
+      <c r="AF43" s="9"/>
+    </row>
+    <row r="44" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A44" s="9"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="9"/>
+      <c r="E44" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F44" s="17" t="s">
+      <c r="F44" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="G44" s="17" t="s">
+      <c r="G44" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H44" s="17" t="s">
+      <c r="H44" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I44" s="15"/>
-      <c r="J44" s="15"/>
-      <c r="K44" s="15"/>
-      <c r="L44" s="15"/>
-      <c r="M44" s="15"/>
-      <c r="N44" s="15"/>
-      <c r="O44" s="15"/>
-      <c r="P44" s="15"/>
-      <c r="Q44" s="15"/>
-      <c r="R44" s="15"/>
-      <c r="S44" s="15"/>
-      <c r="T44" s="15"/>
-      <c r="U44" s="15"/>
-      <c r="V44" s="15"/>
-      <c r="W44" s="15"/>
-      <c r="X44" s="15"/>
-      <c r="Y44" s="15"/>
-      <c r="Z44" s="15"/>
-      <c r="AA44" s="15"/>
-      <c r="AB44" s="15"/>
-      <c r="AC44" s="15"/>
-      <c r="AD44" s="15"/>
-      <c r="AE44" s="15"/>
-      <c r="AF44" s="15"/>
+      <c r="I44" s="9"/>
+      <c r="J44" s="9"/>
+      <c r="K44" s="9"/>
+      <c r="L44" s="9"/>
+      <c r="M44" s="9"/>
+      <c r="N44" s="9"/>
+      <c r="O44" s="9"/>
+      <c r="P44" s="9"/>
+      <c r="Q44" s="9"/>
+      <c r="R44" s="9"/>
+      <c r="S44" s="9"/>
+      <c r="T44" s="9"/>
+      <c r="U44" s="9"/>
+      <c r="V44" s="9"/>
+      <c r="W44" s="9"/>
+      <c r="X44" s="9"/>
+      <c r="Y44" s="9"/>
+      <c r="Z44" s="9"/>
+      <c r="AA44" s="9"/>
+      <c r="AB44" s="9"/>
+      <c r="AC44" s="9"/>
+      <c r="AD44" s="9"/>
+      <c r="AE44" s="9"/>
+      <c r="AF44" s="9"/>
     </row>
     <row r="45" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="4"/>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
       <c r="D45" s="4"/>
-      <c r="E45" s="19" t="s">
+      <c r="E45" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="F45" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="G45" s="14" t="s">
+      <c r="F45" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G45" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H45" s="14" t="s">
+      <c r="H45" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I45" s="4"/>
@@ -2469,131 +2495,131 @@
       <c r="AE45" s="4"/>
       <c r="AF45" s="4"/>
     </row>
-    <row r="46" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="15"/>
-      <c r="B46" s="15"/>
-      <c r="C46" s="15"/>
-      <c r="D46" s="15"/>
-      <c r="E46" s="16" t="s">
+    <row r="46" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="9"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="9"/>
+      <c r="D46" s="9"/>
+      <c r="E46" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F46" s="17" t="s">
+      <c r="F46" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="G46" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H46" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="I46" s="9"/>
+      <c r="J46" s="9"/>
+      <c r="K46" s="9"/>
+      <c r="L46" s="9"/>
+      <c r="M46" s="9"/>
+      <c r="N46" s="9"/>
+      <c r="O46" s="9"/>
+      <c r="P46" s="9"/>
+      <c r="Q46" s="9"/>
+      <c r="R46" s="9"/>
+      <c r="S46" s="9"/>
+      <c r="T46" s="9"/>
+      <c r="U46" s="9"/>
+      <c r="V46" s="9"/>
+      <c r="W46" s="9"/>
+      <c r="X46" s="9"/>
+      <c r="Y46" s="9"/>
+      <c r="Z46" s="9"/>
+      <c r="AA46" s="9"/>
+      <c r="AB46" s="9"/>
+      <c r="AC46" s="9"/>
+      <c r="AD46" s="9"/>
+      <c r="AE46" s="9"/>
+      <c r="AF46" s="9"/>
+    </row>
+    <row r="47" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="F47" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="G46" s="17" t="s">
+      <c r="G47" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H46" s="17" t="s">
+      <c r="H47" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I46" s="15"/>
-      <c r="J46" s="15"/>
-      <c r="K46" s="15"/>
-      <c r="L46" s="15"/>
-      <c r="M46" s="15"/>
-      <c r="N46" s="15"/>
-      <c r="O46" s="15"/>
-      <c r="P46" s="15"/>
-      <c r="Q46" s="15"/>
-      <c r="R46" s="15"/>
-      <c r="S46" s="15"/>
-      <c r="T46" s="15"/>
-      <c r="U46" s="15"/>
-      <c r="V46" s="15"/>
-      <c r="W46" s="15"/>
-      <c r="X46" s="15"/>
-      <c r="Y46" s="15"/>
-      <c r="Z46" s="15"/>
-      <c r="AA46" s="15"/>
-      <c r="AB46" s="15"/>
-      <c r="AC46" s="15"/>
-      <c r="AD46" s="15"/>
-      <c r="AE46" s="15"/>
-      <c r="AF46" s="15"/>
-    </row>
-    <row r="47" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="15"/>
-      <c r="B47" s="15"/>
-      <c r="C47" s="15"/>
-      <c r="D47" s="15"/>
-      <c r="E47" s="16" t="s">
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="9"/>
+      <c r="U47" s="9"/>
+      <c r="V47" s="9"/>
+      <c r="W47" s="9"/>
+      <c r="X47" s="9"/>
+      <c r="Y47" s="9"/>
+      <c r="Z47" s="9"/>
+      <c r="AA47" s="9"/>
+      <c r="AB47" s="9"/>
+      <c r="AC47" s="9"/>
+      <c r="AD47" s="9"/>
+      <c r="AE47" s="9"/>
+      <c r="AF47" s="9"/>
+    </row>
+    <row r="48" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="9"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="9"/>
+      <c r="D48" s="9"/>
+      <c r="E48" s="10" t="s">
         <v>41</v>
       </c>
-      <c r="F47" s="17" t="s">
+      <c r="F48" s="11" t="s">
         <v>73</v>
       </c>
-      <c r="G47" s="17" t="s">
+      <c r="G48" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H47" s="17" t="s">
+      <c r="H48" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I47" s="15"/>
-      <c r="J47" s="15"/>
-      <c r="K47" s="15"/>
-      <c r="L47" s="15"/>
-      <c r="M47" s="15"/>
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
-      <c r="S47" s="15"/>
-      <c r="T47" s="15"/>
-      <c r="U47" s="15"/>
-      <c r="V47" s="15"/>
-      <c r="W47" s="15"/>
-      <c r="X47" s="15"/>
-      <c r="Y47" s="15"/>
-      <c r="Z47" s="15"/>
-      <c r="AA47" s="15"/>
-      <c r="AB47" s="15"/>
-      <c r="AC47" s="15"/>
-      <c r="AD47" s="15"/>
-      <c r="AE47" s="15"/>
-      <c r="AF47" s="15"/>
-    </row>
-    <row r="48" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="15"/>
-      <c r="B48" s="15"/>
-      <c r="C48" s="15"/>
-      <c r="D48" s="15"/>
-      <c r="E48" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="F48" s="17" t="s">
-        <v>74</v>
-      </c>
-      <c r="G48" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H48" s="17" t="s">
-        <v>12</v>
-      </c>
-      <c r="I48" s="15"/>
-      <c r="J48" s="15"/>
-      <c r="K48" s="15"/>
-      <c r="L48" s="15"/>
-      <c r="M48" s="15"/>
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="15"/>
-      <c r="S48" s="15"/>
-      <c r="T48" s="15"/>
-      <c r="U48" s="15"/>
-      <c r="V48" s="15"/>
-      <c r="W48" s="15"/>
-      <c r="X48" s="15"/>
-      <c r="Y48" s="15"/>
-      <c r="Z48" s="15"/>
-      <c r="AA48" s="15"/>
-      <c r="AB48" s="15"/>
-      <c r="AC48" s="15"/>
-      <c r="AD48" s="15"/>
-      <c r="AE48" s="15"/>
-      <c r="AF48" s="15"/>
+      <c r="I48" s="9"/>
+      <c r="J48" s="9"/>
+      <c r="K48" s="9"/>
+      <c r="L48" s="9"/>
+      <c r="M48" s="9"/>
+      <c r="N48" s="9"/>
+      <c r="O48" s="9"/>
+      <c r="P48" s="9"/>
+      <c r="Q48" s="9"/>
+      <c r="R48" s="9"/>
+      <c r="S48" s="9"/>
+      <c r="T48" s="9"/>
+      <c r="U48" s="9"/>
+      <c r="V48" s="9"/>
+      <c r="W48" s="9"/>
+      <c r="X48" s="9"/>
+      <c r="Y48" s="9"/>
+      <c r="Z48" s="9"/>
+      <c r="AA48" s="9"/>
+      <c r="AB48" s="9"/>
+      <c r="AC48" s="9"/>
+      <c r="AD48" s="9"/>
+      <c r="AE48" s="9"/>
+      <c r="AF48" s="9"/>
     </row>
     <row r="49" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="4"/>
@@ -2642,16 +2668,16 @@
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="E50" s="19" t="s">
+      <c r="E50" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F50" s="14" t="s">
+      <c r="F50" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="G50" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="H50" s="14" t="s">
+      <c r="G50" s="8" t="s">
+        <v>67</v>
+      </c>
+      <c r="H50" s="8" t="s">
         <v>13</v>
       </c>
       <c r="I50" s="4"/>
@@ -2679,63 +2705,63 @@
       <c r="AE50" s="4"/>
       <c r="AF50" s="4"/>
     </row>
-    <row r="51" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A51" s="15"/>
-      <c r="B51" s="15"/>
-      <c r="C51" s="15"/>
-      <c r="D51" s="15"/>
-      <c r="E51" s="16" t="s">
+    <row r="51" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A51" s="9"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="9"/>
+      <c r="D51" s="9"/>
+      <c r="E51" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F51" s="17" t="s">
+      <c r="F51" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G51" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="H51" s="17" t="s">
+      <c r="G51" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="H51" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="I51" s="15"/>
-      <c r="J51" s="15"/>
-      <c r="K51" s="15"/>
-      <c r="L51" s="15"/>
-      <c r="M51" s="15"/>
-      <c r="N51" s="15"/>
-      <c r="O51" s="15"/>
-      <c r="P51" s="15"/>
-      <c r="Q51" s="15"/>
-      <c r="R51" s="15"/>
-      <c r="S51" s="15"/>
-      <c r="T51" s="15"/>
-      <c r="U51" s="15"/>
-      <c r="V51" s="15"/>
-      <c r="W51" s="15"/>
-      <c r="X51" s="15"/>
-      <c r="Y51" s="15"/>
-      <c r="Z51" s="15"/>
-      <c r="AA51" s="15"/>
-      <c r="AB51" s="15"/>
-      <c r="AC51" s="15"/>
-      <c r="AD51" s="15"/>
-      <c r="AE51" s="15"/>
-      <c r="AF51" s="15"/>
+      <c r="I51" s="9"/>
+      <c r="J51" s="9"/>
+      <c r="K51" s="9"/>
+      <c r="L51" s="9"/>
+      <c r="M51" s="9"/>
+      <c r="N51" s="9"/>
+      <c r="O51" s="9"/>
+      <c r="P51" s="9"/>
+      <c r="Q51" s="9"/>
+      <c r="R51" s="9"/>
+      <c r="S51" s="9"/>
+      <c r="T51" s="9"/>
+      <c r="U51" s="9"/>
+      <c r="V51" s="9"/>
+      <c r="W51" s="9"/>
+      <c r="X51" s="9"/>
+      <c r="Y51" s="9"/>
+      <c r="Z51" s="9"/>
+      <c r="AA51" s="9"/>
+      <c r="AB51" s="9"/>
+      <c r="AC51" s="9"/>
+      <c r="AD51" s="9"/>
+      <c r="AE51" s="9"/>
+      <c r="AF51" s="9"/>
     </row>
     <row r="52" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="4"/>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
-      <c r="E52" s="19" t="s">
+      <c r="E52" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F52" s="14" t="s">
+      <c r="F52" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="G52" s="14" t="s">
+      <c r="G52" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H52" s="14" t="s">
+      <c r="H52" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I52" s="4"/>
@@ -2763,147 +2789,147 @@
       <c r="AE52" s="4"/>
       <c r="AF52" s="4"/>
     </row>
-    <row r="53" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="15"/>
-      <c r="B53" s="15"/>
-      <c r="C53" s="15"/>
-      <c r="D53" s="15"/>
-      <c r="E53" s="16" t="s">
+    <row r="53" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="9"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="9"/>
+      <c r="D53" s="9"/>
+      <c r="E53" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F53" s="17" t="s">
+      <c r="F53" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="G53" s="17" t="s">
+      <c r="G53" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H53" s="17" t="s">
+      <c r="H53" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I53" s="15"/>
-      <c r="J53" s="15"/>
-      <c r="K53" s="15"/>
-      <c r="L53" s="15"/>
-      <c r="M53" s="15"/>
-      <c r="N53" s="15"/>
-      <c r="O53" s="15"/>
-      <c r="P53" s="15"/>
-      <c r="Q53" s="15"/>
-      <c r="R53" s="15"/>
-      <c r="S53" s="15"/>
-      <c r="T53" s="15"/>
-      <c r="U53" s="15"/>
-      <c r="V53" s="15"/>
-      <c r="W53" s="15"/>
-      <c r="X53" s="15"/>
-      <c r="Y53" s="15"/>
-      <c r="Z53" s="15"/>
-      <c r="AA53" s="15"/>
-      <c r="AB53" s="15"/>
-      <c r="AC53" s="15"/>
-      <c r="AD53" s="15"/>
-      <c r="AE53" s="15"/>
-      <c r="AF53" s="15"/>
-    </row>
-    <row r="54" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="15"/>
-      <c r="B54" s="15"/>
-      <c r="C54" s="15"/>
-      <c r="D54" s="15"/>
-      <c r="E54" s="16" t="s">
+      <c r="I53" s="9"/>
+      <c r="J53" s="9"/>
+      <c r="K53" s="9"/>
+      <c r="L53" s="9"/>
+      <c r="M53" s="9"/>
+      <c r="N53" s="9"/>
+      <c r="O53" s="9"/>
+      <c r="P53" s="9"/>
+      <c r="Q53" s="9"/>
+      <c r="R53" s="9"/>
+      <c r="S53" s="9"/>
+      <c r="T53" s="9"/>
+      <c r="U53" s="9"/>
+      <c r="V53" s="9"/>
+      <c r="W53" s="9"/>
+      <c r="X53" s="9"/>
+      <c r="Y53" s="9"/>
+      <c r="Z53" s="9"/>
+      <c r="AA53" s="9"/>
+      <c r="AB53" s="9"/>
+      <c r="AC53" s="9"/>
+      <c r="AD53" s="9"/>
+      <c r="AE53" s="9"/>
+      <c r="AF53" s="9"/>
+    </row>
+    <row r="54" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="9"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="9"/>
+      <c r="D54" s="9"/>
+      <c r="E54" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F54" s="17" t="s">
+      <c r="F54" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="G54" s="17" t="s">
+      <c r="G54" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H54" s="17" t="s">
+      <c r="H54" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I54" s="15"/>
-      <c r="J54" s="15"/>
-      <c r="K54" s="15"/>
-      <c r="L54" s="15"/>
-      <c r="M54" s="15"/>
-      <c r="N54" s="15"/>
-      <c r="O54" s="15"/>
-      <c r="P54" s="15"/>
-      <c r="Q54" s="15"/>
-      <c r="R54" s="15"/>
-      <c r="S54" s="15"/>
-      <c r="T54" s="15"/>
-      <c r="U54" s="15"/>
-      <c r="V54" s="15"/>
-      <c r="W54" s="15"/>
-      <c r="X54" s="15"/>
-      <c r="Y54" s="15"/>
-      <c r="Z54" s="15"/>
-      <c r="AA54" s="15"/>
-      <c r="AB54" s="15"/>
-      <c r="AC54" s="15"/>
-      <c r="AD54" s="15"/>
-      <c r="AE54" s="15"/>
-      <c r="AF54" s="15"/>
-    </row>
-    <row r="55" spans="1:32" s="18" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A55" s="15"/>
-      <c r="B55" s="15"/>
-      <c r="C55" s="15"/>
-      <c r="D55" s="15"/>
-      <c r="E55" s="16" t="s">
+      <c r="I54" s="9"/>
+      <c r="J54" s="9"/>
+      <c r="K54" s="9"/>
+      <c r="L54" s="9"/>
+      <c r="M54" s="9"/>
+      <c r="N54" s="9"/>
+      <c r="O54" s="9"/>
+      <c r="P54" s="9"/>
+      <c r="Q54" s="9"/>
+      <c r="R54" s="9"/>
+      <c r="S54" s="9"/>
+      <c r="T54" s="9"/>
+      <c r="U54" s="9"/>
+      <c r="V54" s="9"/>
+      <c r="W54" s="9"/>
+      <c r="X54" s="9"/>
+      <c r="Y54" s="9"/>
+      <c r="Z54" s="9"/>
+      <c r="AA54" s="9"/>
+      <c r="AB54" s="9"/>
+      <c r="AC54" s="9"/>
+      <c r="AD54" s="9"/>
+      <c r="AE54" s="9"/>
+      <c r="AF54" s="9"/>
+    </row>
+    <row r="55" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="9"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="9"/>
+      <c r="D55" s="9"/>
+      <c r="E55" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F55" s="17" t="s">
+      <c r="F55" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="G55" s="17" t="s">
-        <v>69</v>
-      </c>
-      <c r="H55" s="17" t="s">
+      <c r="G55" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="H55" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I55" s="15"/>
-      <c r="J55" s="15"/>
-      <c r="K55" s="15"/>
-      <c r="L55" s="15"/>
-      <c r="M55" s="15"/>
-      <c r="N55" s="15"/>
-      <c r="O55" s="15"/>
-      <c r="P55" s="15"/>
-      <c r="Q55" s="15"/>
-      <c r="R55" s="15"/>
-      <c r="S55" s="15"/>
-      <c r="T55" s="15"/>
-      <c r="U55" s="15"/>
-      <c r="V55" s="15"/>
-      <c r="W55" s="15"/>
-      <c r="X55" s="15"/>
-      <c r="Y55" s="15"/>
-      <c r="Z55" s="15"/>
-      <c r="AA55" s="15"/>
-      <c r="AB55" s="15"/>
-      <c r="AC55" s="15"/>
-      <c r="AD55" s="15"/>
-      <c r="AE55" s="15"/>
-      <c r="AF55" s="15"/>
+      <c r="I55" s="9"/>
+      <c r="J55" s="9"/>
+      <c r="K55" s="9"/>
+      <c r="L55" s="9"/>
+      <c r="M55" s="9"/>
+      <c r="N55" s="9"/>
+      <c r="O55" s="9"/>
+      <c r="P55" s="9"/>
+      <c r="Q55" s="9"/>
+      <c r="R55" s="9"/>
+      <c r="S55" s="9"/>
+      <c r="T55" s="9"/>
+      <c r="U55" s="9"/>
+      <c r="V55" s="9"/>
+      <c r="W55" s="9"/>
+      <c r="X55" s="9"/>
+      <c r="Y55" s="9"/>
+      <c r="Z55" s="9"/>
+      <c r="AA55" s="9"/>
+      <c r="AB55" s="9"/>
+      <c r="AC55" s="9"/>
+      <c r="AD55" s="9"/>
+      <c r="AE55" s="9"/>
+      <c r="AF55" s="9"/>
     </row>
     <row r="56" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="4"/>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
-      <c r="E56" s="19" t="s">
+      <c r="E56" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F56" s="14" t="s">
+      <c r="F56" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="G56" s="14" t="s">
+      <c r="G56" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H56" s="14" t="s">
+      <c r="H56" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I56" s="4"/>
@@ -2931,63 +2957,63 @@
       <c r="AE56" s="4"/>
       <c r="AF56" s="4"/>
     </row>
-    <row r="57" spans="1:32" s="18" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="15"/>
-      <c r="B57" s="15"/>
-      <c r="C57" s="15"/>
-      <c r="D57" s="15"/>
-      <c r="E57" s="16" t="s">
+    <row r="57" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="9"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="9"/>
+      <c r="D57" s="9"/>
+      <c r="E57" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F57" s="17" t="s">
+      <c r="F57" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="G57" s="17" t="s">
+      <c r="G57" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H57" s="17" t="s">
+      <c r="H57" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I57" s="15"/>
-      <c r="J57" s="15"/>
-      <c r="K57" s="15"/>
-      <c r="L57" s="15"/>
-      <c r="M57" s="15"/>
-      <c r="N57" s="15"/>
-      <c r="O57" s="15"/>
-      <c r="P57" s="15"/>
-      <c r="Q57" s="15"/>
-      <c r="R57" s="15"/>
-      <c r="S57" s="15"/>
-      <c r="T57" s="15"/>
-      <c r="U57" s="15"/>
-      <c r="V57" s="15"/>
-      <c r="W57" s="15"/>
-      <c r="X57" s="15"/>
-      <c r="Y57" s="15"/>
-      <c r="Z57" s="15"/>
-      <c r="AA57" s="15"/>
-      <c r="AB57" s="15"/>
-      <c r="AC57" s="15"/>
-      <c r="AD57" s="15"/>
-      <c r="AE57" s="15"/>
-      <c r="AF57" s="15"/>
+      <c r="I57" s="9"/>
+      <c r="J57" s="9"/>
+      <c r="K57" s="9"/>
+      <c r="L57" s="9"/>
+      <c r="M57" s="9"/>
+      <c r="N57" s="9"/>
+      <c r="O57" s="9"/>
+      <c r="P57" s="9"/>
+      <c r="Q57" s="9"/>
+      <c r="R57" s="9"/>
+      <c r="S57" s="9"/>
+      <c r="T57" s="9"/>
+      <c r="U57" s="9"/>
+      <c r="V57" s="9"/>
+      <c r="W57" s="9"/>
+      <c r="X57" s="9"/>
+      <c r="Y57" s="9"/>
+      <c r="Z57" s="9"/>
+      <c r="AA57" s="9"/>
+      <c r="AB57" s="9"/>
+      <c r="AC57" s="9"/>
+      <c r="AD57" s="9"/>
+      <c r="AE57" s="9"/>
+      <c r="AF57" s="9"/>
     </row>
     <row r="58" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
-      <c r="E58" s="19" t="s">
+      <c r="E58" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F58" s="14" t="s">
+      <c r="F58" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="G58" s="14" t="s">
+      <c r="G58" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H58" s="14" t="s">
+      <c r="H58" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I58" s="4"/>
@@ -3015,105 +3041,105 @@
       <c r="AE58" s="4"/>
       <c r="AF58" s="4"/>
     </row>
-    <row r="59" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="15"/>
-      <c r="B59" s="15"/>
-      <c r="C59" s="15"/>
-      <c r="D59" s="15"/>
-      <c r="E59" s="16" t="s">
+    <row r="59" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A59" s="9"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="9"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F59" s="17" t="s">
+      <c r="F59" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="G59" s="17" t="s">
+      <c r="G59" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H59" s="17" t="s">
+      <c r="H59" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I59" s="15"/>
-      <c r="J59" s="15"/>
-      <c r="K59" s="15"/>
-      <c r="L59" s="15"/>
-      <c r="M59" s="15"/>
-      <c r="N59" s="15"/>
-      <c r="O59" s="15"/>
-      <c r="P59" s="15"/>
-      <c r="Q59" s="15"/>
-      <c r="R59" s="15"/>
-      <c r="S59" s="15"/>
-      <c r="T59" s="15"/>
-      <c r="U59" s="15"/>
-      <c r="V59" s="15"/>
-      <c r="W59" s="15"/>
-      <c r="X59" s="15"/>
-      <c r="Y59" s="15"/>
-      <c r="Z59" s="15"/>
-      <c r="AA59" s="15"/>
-      <c r="AB59" s="15"/>
-      <c r="AC59" s="15"/>
-      <c r="AD59" s="15"/>
-      <c r="AE59" s="15"/>
-      <c r="AF59" s="15"/>
-    </row>
-    <row r="60" spans="1:32" s="18" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="15"/>
-      <c r="B60" s="15"/>
-      <c r="C60" s="15"/>
-      <c r="D60" s="15"/>
-      <c r="E60" s="16" t="s">
+      <c r="I59" s="9"/>
+      <c r="J59" s="9"/>
+      <c r="K59" s="9"/>
+      <c r="L59" s="9"/>
+      <c r="M59" s="9"/>
+      <c r="N59" s="9"/>
+      <c r="O59" s="9"/>
+      <c r="P59" s="9"/>
+      <c r="Q59" s="9"/>
+      <c r="R59" s="9"/>
+      <c r="S59" s="9"/>
+      <c r="T59" s="9"/>
+      <c r="U59" s="9"/>
+      <c r="V59" s="9"/>
+      <c r="W59" s="9"/>
+      <c r="X59" s="9"/>
+      <c r="Y59" s="9"/>
+      <c r="Z59" s="9"/>
+      <c r="AA59" s="9"/>
+      <c r="AB59" s="9"/>
+      <c r="AC59" s="9"/>
+      <c r="AD59" s="9"/>
+      <c r="AE59" s="9"/>
+      <c r="AF59" s="9"/>
+    </row>
+    <row r="60" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="9"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F60" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="G60" s="17" t="s">
+      <c r="F60" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="G60" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H60" s="17" t="s">
+      <c r="H60" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I60" s="15"/>
-      <c r="J60" s="15"/>
-      <c r="K60" s="15"/>
-      <c r="L60" s="15"/>
-      <c r="M60" s="15"/>
-      <c r="N60" s="15"/>
-      <c r="O60" s="15"/>
-      <c r="P60" s="15"/>
-      <c r="Q60" s="15"/>
-      <c r="R60" s="15"/>
-      <c r="S60" s="15"/>
-      <c r="T60" s="15"/>
-      <c r="U60" s="15"/>
-      <c r="V60" s="15"/>
-      <c r="W60" s="15"/>
-      <c r="X60" s="15"/>
-      <c r="Y60" s="15"/>
-      <c r="Z60" s="15"/>
-      <c r="AA60" s="15"/>
-      <c r="AB60" s="15"/>
-      <c r="AC60" s="15"/>
-      <c r="AD60" s="15"/>
-      <c r="AE60" s="15"/>
-      <c r="AF60" s="15"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9"/>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="9"/>
+      <c r="N60" s="9"/>
+      <c r="O60" s="9"/>
+      <c r="P60" s="9"/>
+      <c r="Q60" s="9"/>
+      <c r="R60" s="9"/>
+      <c r="S60" s="9"/>
+      <c r="T60" s="9"/>
+      <c r="U60" s="9"/>
+      <c r="V60" s="9"/>
+      <c r="W60" s="9"/>
+      <c r="X60" s="9"/>
+      <c r="Y60" s="9"/>
+      <c r="Z60" s="9"/>
+      <c r="AA60" s="9"/>
+      <c r="AB60" s="9"/>
+      <c r="AC60" s="9"/>
+      <c r="AD60" s="9"/>
+      <c r="AE60" s="9"/>
+      <c r="AF60" s="9"/>
     </row>
     <row r="61" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
-      <c r="E61" s="19" t="s">
+      <c r="E61" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F61" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G61" s="14" t="s">
+      <c r="F61" s="8" t="s">
+        <v>62</v>
+      </c>
+      <c r="G61" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H61" s="14" t="s">
+      <c r="H61" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I61" s="4"/>
@@ -3141,63 +3167,63 @@
       <c r="AE61" s="4"/>
       <c r="AF61" s="4"/>
     </row>
-    <row r="62" spans="1:32" s="18" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="15"/>
-      <c r="B62" s="15"/>
-      <c r="C62" s="15"/>
-      <c r="D62" s="15"/>
-      <c r="E62" s="16" t="s">
+    <row r="62" spans="1:32" s="12" customFormat="1" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="9"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="9"/>
+      <c r="D62" s="9"/>
+      <c r="E62" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F62" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="G62" s="17" t="s">
+      <c r="F62" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G62" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H62" s="17" t="s">
+      <c r="H62" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I62" s="15"/>
-      <c r="J62" s="15"/>
-      <c r="K62" s="15"/>
-      <c r="L62" s="15"/>
-      <c r="M62" s="15"/>
-      <c r="N62" s="15"/>
-      <c r="O62" s="15"/>
-      <c r="P62" s="15"/>
-      <c r="Q62" s="15"/>
-      <c r="R62" s="15"/>
-      <c r="S62" s="15"/>
-      <c r="T62" s="15"/>
-      <c r="U62" s="15"/>
-      <c r="V62" s="15"/>
-      <c r="W62" s="15"/>
-      <c r="X62" s="15"/>
-      <c r="Y62" s="15"/>
-      <c r="Z62" s="15"/>
-      <c r="AA62" s="15"/>
-      <c r="AB62" s="15"/>
-      <c r="AC62" s="15"/>
-      <c r="AD62" s="15"/>
-      <c r="AE62" s="15"/>
-      <c r="AF62" s="15"/>
+      <c r="I62" s="9"/>
+      <c r="J62" s="9"/>
+      <c r="K62" s="9"/>
+      <c r="L62" s="9"/>
+      <c r="M62" s="9"/>
+      <c r="N62" s="9"/>
+      <c r="O62" s="9"/>
+      <c r="P62" s="9"/>
+      <c r="Q62" s="9"/>
+      <c r="R62" s="9"/>
+      <c r="S62" s="9"/>
+      <c r="T62" s="9"/>
+      <c r="U62" s="9"/>
+      <c r="V62" s="9"/>
+      <c r="W62" s="9"/>
+      <c r="X62" s="9"/>
+      <c r="Y62" s="9"/>
+      <c r="Z62" s="9"/>
+      <c r="AA62" s="9"/>
+      <c r="AB62" s="9"/>
+      <c r="AC62" s="9"/>
+      <c r="AD62" s="9"/>
+      <c r="AE62" s="9"/>
+      <c r="AF62" s="9"/>
     </row>
     <row r="63" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A63" s="4"/>
       <c r="B63" s="4"/>
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
-      <c r="E63" s="19" t="s">
+      <c r="E63" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="F63" s="14" t="s">
-        <v>65</v>
-      </c>
-      <c r="G63" s="14" t="s">
+      <c r="F63" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="G63" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="H63" s="14" t="s">
+      <c r="H63" s="8" t="s">
         <v>12</v>
       </c>
       <c r="I63" s="4"/>
@@ -3225,89 +3251,89 @@
       <c r="AE63" s="4"/>
       <c r="AF63" s="4"/>
     </row>
-    <row r="64" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="15"/>
-      <c r="B64" s="15"/>
-      <c r="C64" s="15"/>
-      <c r="D64" s="15"/>
-      <c r="E64" s="16" t="s">
+    <row r="64" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A64" s="9"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="9"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F64" s="17" t="s">
+      <c r="F64" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="G64" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="H64" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I64" s="9"/>
+      <c r="J64" s="9"/>
+      <c r="K64" s="9"/>
+      <c r="L64" s="9"/>
+      <c r="M64" s="9"/>
+      <c r="N64" s="9"/>
+      <c r="O64" s="9"/>
+      <c r="P64" s="9"/>
+      <c r="Q64" s="9"/>
+      <c r="R64" s="9"/>
+      <c r="S64" s="9"/>
+      <c r="T64" s="9"/>
+      <c r="U64" s="9"/>
+      <c r="V64" s="9"/>
+      <c r="W64" s="9"/>
+      <c r="X64" s="9"/>
+      <c r="Y64" s="9"/>
+      <c r="Z64" s="9"/>
+      <c r="AA64" s="9"/>
+      <c r="AB64" s="9"/>
+      <c r="AC64" s="9"/>
+      <c r="AD64" s="9"/>
+      <c r="AE64" s="9"/>
+      <c r="AF64" s="9"/>
+    </row>
+    <row r="65" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="F65" s="11" t="s">
         <v>66</v>
       </c>
-      <c r="G64" s="17" t="s">
+      <c r="G65" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="H64" s="17" t="s">
-        <v>13</v>
-      </c>
-      <c r="I64" s="15"/>
-      <c r="J64" s="15"/>
-      <c r="K64" s="15"/>
-      <c r="L64" s="15"/>
-      <c r="M64" s="15"/>
-      <c r="N64" s="15"/>
-      <c r="O64" s="15"/>
-      <c r="P64" s="15"/>
-      <c r="Q64" s="15"/>
-      <c r="R64" s="15"/>
-      <c r="S64" s="15"/>
-      <c r="T64" s="15"/>
-      <c r="U64" s="15"/>
-      <c r="V64" s="15"/>
-      <c r="W64" s="15"/>
-      <c r="X64" s="15"/>
-      <c r="Y64" s="15"/>
-      <c r="Z64" s="15"/>
-      <c r="AA64" s="15"/>
-      <c r="AB64" s="15"/>
-      <c r="AC64" s="15"/>
-      <c r="AD64" s="15"/>
-      <c r="AE64" s="15"/>
-      <c r="AF64" s="15"/>
-    </row>
-    <row r="65" spans="1:32" s="18" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="15"/>
-      <c r="B65" s="15"/>
-      <c r="C65" s="15"/>
-      <c r="D65" s="15"/>
-      <c r="E65" s="16" t="s">
-        <v>44</v>
-      </c>
-      <c r="F65" s="17" t="s">
-        <v>67</v>
-      </c>
-      <c r="G65" s="17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H65" s="17" t="s">
+      <c r="H65" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="I65" s="15"/>
-      <c r="J65" s="15"/>
-      <c r="K65" s="15"/>
-      <c r="L65" s="15"/>
-      <c r="M65" s="15"/>
-      <c r="N65" s="15"/>
-      <c r="O65" s="15"/>
-      <c r="P65" s="15"/>
-      <c r="Q65" s="15"/>
-      <c r="R65" s="15"/>
-      <c r="S65" s="15"/>
-      <c r="T65" s="15"/>
-      <c r="U65" s="15"/>
-      <c r="V65" s="15"/>
-      <c r="W65" s="15"/>
-      <c r="X65" s="15"/>
-      <c r="Y65" s="15"/>
-      <c r="Z65" s="15"/>
-      <c r="AA65" s="15"/>
-      <c r="AB65" s="15"/>
-      <c r="AC65" s="15"/>
-      <c r="AD65" s="15"/>
-      <c r="AE65" s="15"/>
-      <c r="AF65" s="15"/>
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
+      <c r="O65" s="9"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="9"/>
+      <c r="R65" s="9"/>
+      <c r="S65" s="9"/>
+      <c r="T65" s="9"/>
+      <c r="U65" s="9"/>
+      <c r="V65" s="9"/>
+      <c r="W65" s="9"/>
+      <c r="X65" s="9"/>
+      <c r="Y65" s="9"/>
+      <c r="Z65" s="9"/>
+      <c r="AA65" s="9"/>
+      <c r="AB65" s="9"/>
+      <c r="AC65" s="9"/>
+      <c r="AD65" s="9"/>
+      <c r="AE65" s="9"/>
+      <c r="AF65" s="9"/>
     </row>
     <row r="66" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A66" s="4"/>
@@ -7073,6 +7099,6 @@
     <hyperlink ref="E70" location="_ftnref4" display="_ftnref4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Incidencias Resueltas y Requerimientos Funcionales
</commit_message>
<xml_diff>
--- a/Requerimientos funcionales/Requerimientos Funcionales.xlsx
+++ b/Requerimientos funcionales/Requerimientos Funcionales.xlsx
@@ -10,10 +10,10 @@
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_ftn1" localSheetId="0">Hoja1!$B$126</definedName>
-    <definedName name="_ftn2" localSheetId="0">Hoja1!$B$127</definedName>
-    <definedName name="_ftn3" localSheetId="0">Hoja1!$B$134</definedName>
-    <definedName name="_ftn4" localSheetId="0">Hoja1!$B$135</definedName>
+    <definedName name="_ftn1" localSheetId="0">Hoja1!$B$125</definedName>
+    <definedName name="_ftn2" localSheetId="0">Hoja1!$B$126</definedName>
+    <definedName name="_ftn3" localSheetId="0">Hoja1!$B$133</definedName>
+    <definedName name="_ftn4" localSheetId="0">Hoja1!$B$134</definedName>
     <definedName name="_ftnref1" localSheetId="0">Hoja1!$B$7</definedName>
     <definedName name="_ftnref2" localSheetId="0">Hoja1!$C$7</definedName>
   </definedNames>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="525" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="523" uniqueCount="271">
   <si>
     <t>Especificación de Requerimientos Funcionales</t>
   </si>
@@ -144,12 +144,6 @@
     <t>RF-GU 1.7</t>
   </si>
   <si>
-    <t>Ingresar Contraseña:  debe contener al menos 6 caracteres, mayúsculas, minúsculas y al menos un número o carácter especial</t>
-  </si>
-  <si>
-    <t>Ingresar Usuario en el formulario : nombre de usuario unico escrito solo en letras minúsculas</t>
-  </si>
-  <si>
     <t>Ingresar Cedula: se debe ingresar un numero de 9 digitos</t>
   </si>
   <si>
@@ -249,9 +243,6 @@
     <t>RF- CP 5.2</t>
   </si>
   <si>
-    <t>El precio se calcula sobre el precio costo, una vez ingresado el producto en el inventario</t>
-  </si>
-  <si>
     <t>El porcentaje añadido al precio por producto varía según la categoría</t>
   </si>
   <si>
@@ -297,9 +288,6 @@
     <t>RF-CP 6.2</t>
   </si>
   <si>
-    <t>Cada categoría de descuento tiene un codigo que la identifica</t>
-  </si>
-  <si>
     <t xml:space="preserve"> Envío de pedidos</t>
   </si>
   <si>
@@ -708,15 +696,6 @@
     <t>RF- GC 20.1</t>
   </si>
   <si>
-    <t>Ingresar el nombre completo del cliente</t>
-  </si>
-  <si>
-    <t>Ingresar apellidos del cliente</t>
-  </si>
-  <si>
-    <t>Ingresar la cédula del cliente con un formato de 8 dígitos</t>
-  </si>
-  <si>
     <t>Ingresar el email o sitio web del proveedor, si éste cuenta con eso</t>
   </si>
   <si>
@@ -756,33 +735,15 @@
     <t>RF- GC 20.7</t>
   </si>
   <si>
-    <t xml:space="preserve">Ingresar el Nombre completo </t>
-  </si>
-  <si>
-    <t>Ingresar los dos Apellidos</t>
-  </si>
-  <si>
     <t>RF-GU 1.8</t>
   </si>
   <si>
     <t>RF-GU 1.9</t>
   </si>
   <si>
-    <t xml:space="preserve">El sistema no puede guardar ninguna contraseña, para mayor seguridad </t>
-  </si>
-  <si>
     <t>Una vez que se cierre el navegador o se apaga el equipo, la sesión se debe cerrar</t>
   </si>
   <si>
-    <t>RF-GU 2.4</t>
-  </si>
-  <si>
-    <t>RF-GU 2.5</t>
-  </si>
-  <si>
-    <t>Validacion del Rol de usuarios (Vendedor o Administrador): se debe indicar qué tipo de usuario</t>
-  </si>
-  <si>
     <t>Si el usuario es Vendedor: solo tiene permiso de vender productos, generar facturas y registrar clientes</t>
   </si>
   <si>
@@ -801,9 +762,6 @@
     <t>RF-CP 3.1.4</t>
   </si>
   <si>
-    <t>Se debe ingresar el nombre de la categoría</t>
-  </si>
-  <si>
     <t>Ingresar la descripción del producto</t>
   </si>
   <si>
@@ -828,9 +786,6 @@
     <t>Indicar el método de pago, si será en efectivo, en línea, etc</t>
   </si>
   <si>
-    <t>OE</t>
-  </si>
-  <si>
     <t>Control Clientes Frecuentes</t>
   </si>
   <si>
@@ -877,6 +832,45 @@
   </si>
   <si>
     <t>Tener registrado las fechas de compras generadas por estos clientes para futuros pedidos en ciertas épocas</t>
+  </si>
+  <si>
+    <t>Ingresar el Nombre completo: se permiten caracteres del alfabeto</t>
+  </si>
+  <si>
+    <t>Ingresar los dos Apellidos: se permiten caracteres del alfabeto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Ingresar Usuario en el formulario : nombre de usuario unico escrito con caracteres alfanumericos </t>
+  </si>
+  <si>
+    <t>Ingresar Contraseña:  debe contener al menos 6 caracteres, mayúsculas, minúsculas y al menos un número o signo especial</t>
+  </si>
+  <si>
+    <t>El campo para la contraseña debe estar oculta al usuario, con un formato de máscara (*******)</t>
+  </si>
+  <si>
+    <t>RF-GU 2.1 .1</t>
+  </si>
+  <si>
+    <t>RF-GU 2.1.2</t>
+  </si>
+  <si>
+    <t>Se debe ingresar el nombre de la categoría: con caracteres alfanumericos</t>
+  </si>
+  <si>
+    <t>El precio de venta se calcula sobre el precio costo, una vez ingresado el producto en el inventario</t>
+  </si>
+  <si>
+    <t>Cada categoría de descuento tiene un codigo numérico que la identifica</t>
+  </si>
+  <si>
+    <t>Ingresar el nombre completo del cliente con caracteres alfabeticos</t>
+  </si>
+  <si>
+    <t>Ingresar apellidos del cliente con caracteres alfabeticos</t>
+  </si>
+  <si>
+    <t>Ingresar la cédula del cliente con un formato de 9 dígitos</t>
   </si>
 </sst>
 </file>
@@ -1389,10 +1383,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AF244"/>
+  <dimension ref="A1:AF243"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+    <sheetView tabSelected="1" topLeftCell="A134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F141" sqref="F141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1647,7 +1641,7 @@
         <v>21</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>232</v>
+        <v>258</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>9</v>
@@ -1689,7 +1683,7 @@
         <v>22</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>233</v>
+        <v>259</v>
       </c>
       <c r="G13" s="11" t="s">
         <v>16</v>
@@ -1731,7 +1725,7 @@
         <v>23</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>29</v>
+        <v>260</v>
       </c>
       <c r="G14" s="11" t="s">
         <v>9</v>
@@ -1773,7 +1767,7 @@
         <v>24</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>28</v>
+        <v>261</v>
       </c>
       <c r="G15" s="11" t="s">
         <v>9</v>
@@ -1815,7 +1809,7 @@
         <v>25</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>9</v>
@@ -1857,7 +1851,7 @@
         <v>26</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="G17" s="11" t="s">
         <v>16</v>
@@ -1899,7 +1893,7 @@
         <v>27</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="G18" s="11" t="s">
         <v>17</v>
@@ -1938,10 +1932,10 @@
       <c r="C19" s="9"/>
       <c r="D19" s="9"/>
       <c r="E19" s="10" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="G19" s="11" t="s">
         <v>16</v>
@@ -1980,10 +1974,10 @@
       <c r="C20" s="9"/>
       <c r="D20" s="9"/>
       <c r="E20" s="10" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>221</v>
+        <v>214</v>
       </c>
       <c r="G20" s="11" t="s">
         <v>17</v>
@@ -2022,10 +2016,10 @@
       <c r="C21" s="4"/>
       <c r="D21" s="4"/>
       <c r="E21" s="13" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F21" s="8" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="G21" s="8" t="s">
         <v>9</v>
@@ -2064,10 +2058,10 @@
       <c r="C22" s="9"/>
       <c r="D22" s="9"/>
       <c r="E22" s="10" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="F22" s="11" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G22" s="11" t="s">
         <v>9</v>
@@ -2100,19 +2094,23 @@
       <c r="AE22" s="9"/>
       <c r="AF22" s="9"/>
     </row>
-    <row r="23" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
       <c r="B23" s="9"/>
       <c r="C23" s="9"/>
       <c r="D23" s="9"/>
       <c r="E23" s="10" t="s">
-        <v>37</v>
+        <v>263</v>
       </c>
       <c r="F23" s="11" t="s">
-        <v>236</v>
-      </c>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
+        <v>229</v>
+      </c>
+      <c r="G23" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="I23" s="9"/>
       <c r="J23" s="9"/>
       <c r="K23" s="9"/>
@@ -2144,16 +2142,16 @@
       <c r="C24" s="9"/>
       <c r="D24" s="9"/>
       <c r="E24" s="10" t="s">
-        <v>38</v>
+        <v>264</v>
       </c>
       <c r="F24" s="11" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
       <c r="G24" s="11" t="s">
         <v>9</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I24" s="9"/>
       <c r="J24" s="9"/>
@@ -2186,16 +2184,16 @@
       <c r="C25" s="9"/>
       <c r="D25" s="9"/>
       <c r="E25" s="10" t="s">
-        <v>238</v>
+        <v>35</v>
       </c>
       <c r="F25" s="11" t="s">
-        <v>240</v>
+        <v>262</v>
       </c>
       <c r="G25" s="11" t="s">
         <v>9</v>
       </c>
       <c r="H25" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I25" s="9"/>
       <c r="J25" s="9"/>
@@ -2222,22 +2220,22 @@
       <c r="AE25" s="9"/>
       <c r="AF25" s="9"/>
     </row>
-    <row r="26" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="9"/>
       <c r="B26" s="9"/>
       <c r="C26" s="9"/>
       <c r="D26" s="9"/>
       <c r="E26" s="10" t="s">
-        <v>239</v>
+        <v>36</v>
       </c>
       <c r="F26" s="11" t="s">
-        <v>242</v>
+        <v>227</v>
       </c>
       <c r="G26" s="11" t="s">
         <v>9</v>
       </c>
       <c r="H26" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I26" s="9"/>
       <c r="J26" s="9"/>
@@ -2264,61 +2262,57 @@
       <c r="AE26" s="9"/>
       <c r="AF26" s="9"/>
     </row>
-    <row r="27" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="9"/>
-      <c r="B27" s="9"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="10" t="s">
-        <v>239</v>
-      </c>
-      <c r="F27" s="11" t="s">
-        <v>241</v>
-      </c>
-      <c r="G27" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H27" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I27" s="9"/>
-      <c r="J27" s="9"/>
-      <c r="K27" s="9"/>
-      <c r="L27" s="9"/>
-      <c r="M27" s="9"/>
-      <c r="N27" s="9"/>
-      <c r="O27" s="9"/>
-      <c r="P27" s="9"/>
-      <c r="Q27" s="9"/>
-      <c r="R27" s="9"/>
-      <c r="S27" s="9"/>
-      <c r="T27" s="9"/>
-      <c r="U27" s="9"/>
-      <c r="V27" s="9"/>
-      <c r="W27" s="9"/>
-      <c r="X27" s="9"/>
-      <c r="Y27" s="9"/>
-      <c r="Z27" s="9"/>
-      <c r="AA27" s="9"/>
-      <c r="AB27" s="9"/>
-      <c r="AC27" s="9"/>
-      <c r="AD27" s="9"/>
-      <c r="AE27" s="9"/>
-      <c r="AF27" s="9"/>
+    <row r="27" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="G27" s="2"/>
+      <c r="H27" s="2"/>
+      <c r="I27" s="4"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="4"/>
+      <c r="L27" s="4"/>
+      <c r="M27" s="4"/>
+      <c r="N27" s="4"/>
+      <c r="O27" s="4"/>
+      <c r="P27" s="4"/>
+      <c r="Q27" s="4"/>
+      <c r="R27" s="4"/>
+      <c r="S27" s="4"/>
+      <c r="T27" s="4"/>
+      <c r="U27" s="4"/>
+      <c r="V27" s="4"/>
+      <c r="W27" s="4"/>
+      <c r="X27" s="4"/>
+      <c r="Y27" s="4"/>
+      <c r="Z27" s="4"/>
+      <c r="AA27" s="4"/>
+      <c r="AB27" s="4"/>
+      <c r="AC27" s="4"/>
+      <c r="AD27" s="4"/>
+      <c r="AE27" s="4"/>
+      <c r="AF27" s="4"/>
     </row>
     <row r="28" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="4"/>
       <c r="D28" s="4"/>
-      <c r="E28" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="F28" s="2" t="s">
+      <c r="E28" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2"/>
+      <c r="F28" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="G28" s="13"/>
+      <c r="H28" s="13"/>
       <c r="I28" s="4"/>
       <c r="J28" s="4"/>
       <c r="K28" s="4"/>
@@ -2349,14 +2343,18 @@
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
       <c r="D29" s="4"/>
-      <c r="E29" s="13" t="s">
-        <v>41</v>
-      </c>
-      <c r="F29" s="13" t="s">
+      <c r="E29" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="F29" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>9</v>
+      </c>
+      <c r="H29" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="I29" s="4"/>
       <c r="J29" s="4"/>
       <c r="K29" s="4"/>
@@ -2391,13 +2389,13 @@
         <v>44</v>
       </c>
       <c r="F30" s="11" t="s">
-        <v>40</v>
+        <v>265</v>
       </c>
       <c r="G30" s="10" t="s">
         <v>9</v>
       </c>
       <c r="H30" s="10" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I30" s="4"/>
       <c r="J30" s="4"/>
@@ -2424,22 +2422,22 @@
       <c r="AE30" s="4"/>
       <c r="AF30" s="4"/>
     </row>
-    <row r="31" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:32" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
       <c r="D31" s="4"/>
       <c r="E31" s="10" t="s">
-        <v>46</v>
-      </c>
-      <c r="F31" s="11" t="s">
-        <v>247</v>
+        <v>43</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>231</v>
       </c>
       <c r="G31" s="10" t="s">
         <v>9</v>
       </c>
       <c r="H31" s="10" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I31" s="4"/>
       <c r="J31" s="4"/>
@@ -2466,7 +2464,7 @@
       <c r="AE31" s="4"/>
       <c r="AF31" s="4"/>
     </row>
-    <row r="32" spans="1:32" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -2475,7 +2473,7 @@
         <v>45</v>
       </c>
       <c r="F32" s="10" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="G32" s="10" t="s">
         <v>9</v>
@@ -2508,16 +2506,16 @@
       <c r="AE32" s="4"/>
       <c r="AF32" s="4"/>
     </row>
-    <row r="33" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:32" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
       <c r="D33" s="4"/>
       <c r="E33" s="10" t="s">
-        <v>47</v>
-      </c>
-      <c r="F33" s="10" t="s">
-        <v>245</v>
+        <v>45</v>
+      </c>
+      <c r="F33" s="11" t="s">
+        <v>230</v>
       </c>
       <c r="G33" s="10" t="s">
         <v>9</v>
@@ -2550,21 +2548,21 @@
       <c r="AE33" s="4"/>
       <c r="AF33" s="4"/>
     </row>
-    <row r="34" spans="1:32" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
       <c r="D34" s="4"/>
       <c r="E34" s="10" t="s">
-        <v>47</v>
+        <v>233</v>
       </c>
       <c r="F34" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="G34" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="G34" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="10" t="s">
+      <c r="H34" s="11" t="s">
         <v>11</v>
       </c>
       <c r="I34" s="4"/>
@@ -2598,7 +2596,7 @@
       <c r="C35" s="4"/>
       <c r="D35" s="4"/>
       <c r="E35" s="10" t="s">
-        <v>246</v>
+        <v>47</v>
       </c>
       <c r="F35" s="11" t="s">
         <v>48</v>
@@ -2607,7 +2605,7 @@
         <v>9</v>
       </c>
       <c r="H35" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I35" s="4"/>
       <c r="J35" s="4"/>
@@ -2643,10 +2641,10 @@
         <v>49</v>
       </c>
       <c r="F36" s="11" t="s">
-        <v>50</v>
+        <v>234</v>
       </c>
       <c r="G36" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H36" s="11" t="s">
         <v>10</v>
@@ -2682,10 +2680,10 @@
       <c r="C37" s="4"/>
       <c r="D37" s="4"/>
       <c r="E37" s="10" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F37" s="11" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="G37" s="11" t="s">
         <v>16</v>
@@ -2724,13 +2722,13 @@
       <c r="C38" s="4"/>
       <c r="D38" s="4"/>
       <c r="E38" s="10" t="s">
-        <v>52</v>
+        <v>68</v>
       </c>
       <c r="F38" s="11" t="s">
-        <v>249</v>
+        <v>67</v>
       </c>
       <c r="G38" s="11" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H38" s="11" t="s">
         <v>10</v>
@@ -2766,15 +2764,15 @@
       <c r="C39" s="4"/>
       <c r="D39" s="4"/>
       <c r="E39" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>70</v>
-      </c>
-      <c r="G39" s="11" t="s">
+        <v>236</v>
+      </c>
+      <c r="G39" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H39" s="11" t="s">
+      <c r="H39" s="10" t="s">
         <v>10</v>
       </c>
       <c r="I39" s="4"/>
@@ -2808,17 +2806,13 @@
       <c r="C40" s="4"/>
       <c r="D40" s="4"/>
       <c r="E40" s="10" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>250</v>
-      </c>
-      <c r="G40" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="H40" s="10" t="s">
-        <v>10</v>
-      </c>
+        <v>69</v>
+      </c>
+      <c r="G40" s="11"/>
+      <c r="H40" s="11"/>
       <c r="I40" s="4"/>
       <c r="J40" s="4"/>
       <c r="K40" s="4"/>
@@ -2844,19 +2838,23 @@
       <c r="AE40" s="4"/>
       <c r="AF40" s="4"/>
     </row>
-    <row r="41" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
       <c r="D41" s="4"/>
       <c r="E41" s="10" t="s">
-        <v>71</v>
+        <v>256</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>72</v>
-      </c>
-      <c r="G41" s="11"/>
-      <c r="H41" s="11"/>
+        <v>255</v>
+      </c>
+      <c r="G41" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H41" s="11" t="s">
+        <v>10</v>
+      </c>
       <c r="I41" s="4"/>
       <c r="J41" s="4"/>
       <c r="K41" s="4"/>
@@ -2882,21 +2880,21 @@
       <c r="AE41" s="4"/>
       <c r="AF41" s="4"/>
     </row>
-    <row r="42" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
-      <c r="E42" s="10" t="s">
-        <v>271</v>
-      </c>
-      <c r="F42" s="11" t="s">
-        <v>270</v>
-      </c>
-      <c r="G42" s="11" t="s">
+      <c r="E42" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="F42" s="8" t="s">
+        <v>52</v>
+      </c>
+      <c r="G42" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H42" s="11" t="s">
+      <c r="H42" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I42" s="4"/>
@@ -2924,49 +2922,49 @@
       <c r="AE42" s="4"/>
       <c r="AF42" s="4"/>
     </row>
-    <row r="43" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A43" s="4"/>
-      <c r="B43" s="4"/>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="13" t="s">
+    <row r="43" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A43" s="9"/>
+      <c r="B43" s="9"/>
+      <c r="C43" s="9"/>
+      <c r="D43" s="9"/>
+      <c r="E43" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="F43" s="8" t="s">
+      <c r="F43" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="G43" s="8" t="s">
+      <c r="G43" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H43" s="8" t="s">
+      <c r="H43" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I43" s="4"/>
-      <c r="J43" s="4"/>
-      <c r="K43" s="4"/>
-      <c r="L43" s="4"/>
-      <c r="M43" s="4"/>
-      <c r="N43" s="4"/>
-      <c r="O43" s="4"/>
-      <c r="P43" s="4"/>
-      <c r="Q43" s="4"/>
-      <c r="R43" s="4"/>
-      <c r="S43" s="4"/>
-      <c r="T43" s="4"/>
-      <c r="U43" s="4"/>
-      <c r="V43" s="4"/>
-      <c r="W43" s="4"/>
-      <c r="X43" s="4"/>
-      <c r="Y43" s="4"/>
-      <c r="Z43" s="4"/>
-      <c r="AA43" s="4"/>
-      <c r="AB43" s="4"/>
-      <c r="AC43" s="4"/>
-      <c r="AD43" s="4"/>
-      <c r="AE43" s="4"/>
-      <c r="AF43" s="4"/>
-    </row>
-    <row r="44" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I43" s="9"/>
+      <c r="J43" s="9"/>
+      <c r="K43" s="9"/>
+      <c r="L43" s="9"/>
+      <c r="M43" s="9"/>
+      <c r="N43" s="9"/>
+      <c r="O43" s="9"/>
+      <c r="P43" s="9"/>
+      <c r="Q43" s="9"/>
+      <c r="R43" s="9"/>
+      <c r="S43" s="9"/>
+      <c r="T43" s="9"/>
+      <c r="U43" s="9"/>
+      <c r="V43" s="9"/>
+      <c r="W43" s="9"/>
+      <c r="X43" s="9"/>
+      <c r="Y43" s="9"/>
+      <c r="Z43" s="9"/>
+      <c r="AA43" s="9"/>
+      <c r="AB43" s="9"/>
+      <c r="AC43" s="9"/>
+      <c r="AD43" s="9"/>
+      <c r="AE43" s="9"/>
+      <c r="AF43" s="9"/>
+    </row>
+    <row r="44" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="9"/>
       <c r="B44" s="9"/>
       <c r="C44" s="9"/>
@@ -3014,10 +3012,10 @@
       <c r="C45" s="9"/>
       <c r="D45" s="9"/>
       <c r="E45" s="10" t="s">
-        <v>57</v>
+        <v>237</v>
       </c>
       <c r="F45" s="11" t="s">
-        <v>58</v>
+        <v>238</v>
       </c>
       <c r="G45" s="11" t="s">
         <v>9</v>
@@ -3050,100 +3048,100 @@
       <c r="AE45" s="9"/>
       <c r="AF45" s="9"/>
     </row>
-    <row r="46" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="9"/>
-      <c r="B46" s="9"/>
-      <c r="C46" s="9"/>
-      <c r="D46" s="9"/>
-      <c r="E46" s="10" t="s">
-        <v>251</v>
-      </c>
-      <c r="F46" s="11" t="s">
-        <v>252</v>
-      </c>
-      <c r="G46" s="11" t="s">
+    <row r="46" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="4"/>
+      <c r="B46" s="4"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="4"/>
+      <c r="E46" s="13" t="s">
+        <v>58</v>
+      </c>
+      <c r="F46" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="G46" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H46" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I46" s="4"/>
+      <c r="J46" s="4"/>
+      <c r="K46" s="4"/>
+      <c r="L46" s="4"/>
+      <c r="M46" s="4"/>
+      <c r="N46" s="4"/>
+      <c r="O46" s="4"/>
+      <c r="P46" s="4"/>
+      <c r="Q46" s="4"/>
+      <c r="R46" s="4"/>
+      <c r="S46" s="4"/>
+      <c r="T46" s="4"/>
+      <c r="U46" s="4"/>
+      <c r="V46" s="4"/>
+      <c r="W46" s="4"/>
+      <c r="X46" s="4"/>
+      <c r="Y46" s="4"/>
+      <c r="Z46" s="4"/>
+      <c r="AA46" s="4"/>
+      <c r="AB46" s="4"/>
+      <c r="AC46" s="4"/>
+      <c r="AD46" s="4"/>
+      <c r="AE46" s="4"/>
+      <c r="AF46" s="4"/>
+    </row>
+    <row r="47" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A47" s="9"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="9"/>
+      <c r="D47" s="9"/>
+      <c r="E47" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="F47" s="11" t="s">
+        <v>266</v>
+      </c>
+      <c r="G47" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H46" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I46" s="9"/>
-      <c r="J46" s="9"/>
-      <c r="K46" s="9"/>
-      <c r="L46" s="9"/>
-      <c r="M46" s="9"/>
-      <c r="N46" s="9"/>
-      <c r="O46" s="9"/>
-      <c r="P46" s="9"/>
-      <c r="Q46" s="9"/>
-      <c r="R46" s="9"/>
-      <c r="S46" s="9"/>
-      <c r="T46" s="9"/>
-      <c r="U46" s="9"/>
-      <c r="V46" s="9"/>
-      <c r="W46" s="9"/>
-      <c r="X46" s="9"/>
-      <c r="Y46" s="9"/>
-      <c r="Z46" s="9"/>
-      <c r="AA46" s="9"/>
-      <c r="AB46" s="9"/>
-      <c r="AC46" s="9"/>
-      <c r="AD46" s="9"/>
-      <c r="AE46" s="9"/>
-      <c r="AF46" s="9"/>
-    </row>
-    <row r="47" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="4"/>
-      <c r="B47" s="4"/>
-      <c r="C47" s="4"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="13" t="s">
-        <v>60</v>
-      </c>
-      <c r="F47" s="8" t="s">
-        <v>59</v>
-      </c>
-      <c r="G47" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H47" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I47" s="4"/>
-      <c r="J47" s="4"/>
-      <c r="K47" s="4"/>
-      <c r="L47" s="4"/>
-      <c r="M47" s="4"/>
-      <c r="N47" s="4"/>
-      <c r="O47" s="4"/>
-      <c r="P47" s="4"/>
-      <c r="Q47" s="4"/>
-      <c r="R47" s="4"/>
-      <c r="S47" s="4"/>
-      <c r="T47" s="4"/>
-      <c r="U47" s="4"/>
-      <c r="V47" s="4"/>
-      <c r="W47" s="4"/>
-      <c r="X47" s="4"/>
-      <c r="Y47" s="4"/>
-      <c r="Z47" s="4"/>
-      <c r="AA47" s="4"/>
-      <c r="AB47" s="4"/>
-      <c r="AC47" s="4"/>
-      <c r="AD47" s="4"/>
-      <c r="AE47" s="4"/>
-      <c r="AF47" s="4"/>
-    </row>
-    <row r="48" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="H47" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I47" s="9"/>
+      <c r="J47" s="9"/>
+      <c r="K47" s="9"/>
+      <c r="L47" s="9"/>
+      <c r="M47" s="9"/>
+      <c r="N47" s="9"/>
+      <c r="O47" s="9"/>
+      <c r="P47" s="9"/>
+      <c r="Q47" s="9"/>
+      <c r="R47" s="9"/>
+      <c r="S47" s="9"/>
+      <c r="T47" s="9"/>
+      <c r="U47" s="9"/>
+      <c r="V47" s="9"/>
+      <c r="W47" s="9"/>
+      <c r="X47" s="9"/>
+      <c r="Y47" s="9"/>
+      <c r="Z47" s="9"/>
+      <c r="AA47" s="9"/>
+      <c r="AB47" s="9"/>
+      <c r="AC47" s="9"/>
+      <c r="AD47" s="9"/>
+      <c r="AE47" s="9"/>
+      <c r="AF47" s="9"/>
+    </row>
+    <row r="48" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="9"/>
       <c r="B48" s="9"/>
       <c r="C48" s="9"/>
       <c r="D48" s="9"/>
       <c r="E48" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="F48" s="11" t="s">
         <v>61</v>
-      </c>
-      <c r="F48" s="11" t="s">
-        <v>63</v>
       </c>
       <c r="G48" s="11" t="s">
         <v>9</v>
@@ -3176,16 +3174,16 @@
       <c r="AE48" s="9"/>
       <c r="AF48" s="9"/>
     </row>
-    <row r="49" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="9"/>
       <c r="B49" s="9"/>
       <c r="C49" s="9"/>
       <c r="D49" s="9"/>
       <c r="E49" s="10" t="s">
-        <v>62</v>
+        <v>239</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>64</v>
+        <v>240</v>
       </c>
       <c r="G49" s="11" t="s">
         <v>9</v>
@@ -3218,22 +3216,22 @@
       <c r="AE49" s="9"/>
       <c r="AF49" s="9"/>
     </row>
-    <row r="50" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="9"/>
       <c r="B50" s="9"/>
       <c r="C50" s="9"/>
       <c r="D50" s="9"/>
-      <c r="E50" s="10" t="s">
-        <v>253</v>
-      </c>
-      <c r="F50" s="11" t="s">
-        <v>254</v>
-      </c>
-      <c r="G50" s="11" t="s">
+      <c r="E50" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="F50" s="8" t="s">
+        <v>70</v>
+      </c>
+      <c r="G50" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H50" s="11" t="s">
-        <v>11</v>
+      <c r="H50" s="8" t="s">
+        <v>10</v>
       </c>
       <c r="I50" s="9"/>
       <c r="J50" s="9"/>
@@ -3265,17 +3263,17 @@
       <c r="B51" s="9"/>
       <c r="C51" s="9"/>
       <c r="D51" s="9"/>
-      <c r="E51" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="F51" s="8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G51" s="8" t="s">
+      <c r="E51" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="F51" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="G51" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="H51" s="8" t="s">
-        <v>10</v>
+      <c r="H51" s="10" t="s">
+        <v>11</v>
       </c>
       <c r="I51" s="9"/>
       <c r="J51" s="9"/>
@@ -3302,22 +3300,22 @@
       <c r="AE51" s="9"/>
       <c r="AF51" s="9"/>
     </row>
-    <row r="52" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="9"/>
       <c r="B52" s="9"/>
       <c r="C52" s="9"/>
       <c r="D52" s="9"/>
       <c r="E52" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="F52" s="10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G52" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="F52" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="G52" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H52" s="10" t="s">
-        <v>11</v>
+      <c r="H52" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="I52" s="9"/>
       <c r="J52" s="9"/>
@@ -3350,10 +3348,10 @@
       <c r="C53" s="9"/>
       <c r="D53" s="9"/>
       <c r="E53" s="14" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="F53" s="11" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="G53" s="11" t="s">
         <v>9</v>
@@ -3386,16 +3384,16 @@
       <c r="AE53" s="9"/>
       <c r="AF53" s="9"/>
     </row>
-    <row r="54" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A54" s="9"/>
       <c r="B54" s="9"/>
       <c r="C54" s="9"/>
       <c r="D54" s="9"/>
       <c r="E54" s="14" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="F54" s="11" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="G54" s="11" t="s">
         <v>9</v>
@@ -3428,22 +3426,22 @@
       <c r="AE54" s="9"/>
       <c r="AF54" s="9"/>
     </row>
-    <row r="55" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
       <c r="B55" s="9"/>
       <c r="C55" s="9"/>
       <c r="D55" s="9"/>
       <c r="E55" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="F55" s="11" t="s">
-        <v>68</v>
+        <v>267</v>
       </c>
       <c r="G55" s="11" t="s">
         <v>9</v>
       </c>
       <c r="H55" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I55" s="9"/>
       <c r="J55" s="9"/>
@@ -3470,61 +3468,61 @@
       <c r="AE55" s="9"/>
       <c r="AF55" s="9"/>
     </row>
-    <row r="56" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A56" s="9"/>
-      <c r="B56" s="9"/>
-      <c r="C56" s="9"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="14" t="s">
-        <v>78</v>
-      </c>
-      <c r="F56" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="G56" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H56" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I56" s="9"/>
-      <c r="J56" s="9"/>
-      <c r="K56" s="9"/>
-      <c r="L56" s="9"/>
-      <c r="M56" s="9"/>
-      <c r="N56" s="9"/>
-      <c r="O56" s="9"/>
-      <c r="P56" s="9"/>
-      <c r="Q56" s="9"/>
-      <c r="R56" s="9"/>
-      <c r="S56" s="9"/>
-      <c r="T56" s="9"/>
-      <c r="U56" s="9"/>
-      <c r="V56" s="9"/>
-      <c r="W56" s="9"/>
-      <c r="X56" s="9"/>
-      <c r="Y56" s="9"/>
-      <c r="Z56" s="9"/>
-      <c r="AA56" s="9"/>
-      <c r="AB56" s="9"/>
-      <c r="AC56" s="9"/>
-      <c r="AD56" s="9"/>
-      <c r="AE56" s="9"/>
-      <c r="AF56" s="9"/>
+    <row r="56" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="4"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="4"/>
+      <c r="D56" s="4"/>
+      <c r="E56" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="G56" s="2"/>
+      <c r="H56" s="2"/>
+      <c r="I56" s="4"/>
+      <c r="J56" s="4"/>
+      <c r="K56" s="4"/>
+      <c r="L56" s="4"/>
+      <c r="M56" s="4"/>
+      <c r="N56" s="4"/>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4"/>
+      <c r="Q56" s="4"/>
+      <c r="R56" s="4"/>
+      <c r="S56" s="4"/>
+      <c r="T56" s="4"/>
+      <c r="U56" s="4"/>
+      <c r="V56" s="4"/>
+      <c r="W56" s="4"/>
+      <c r="X56" s="4"/>
+      <c r="Y56" s="4"/>
+      <c r="Z56" s="4"/>
+      <c r="AA56" s="4"/>
+      <c r="AB56" s="4"/>
+      <c r="AC56" s="4"/>
+      <c r="AD56" s="4"/>
+      <c r="AE56" s="4"/>
+      <c r="AF56" s="4"/>
     </row>
     <row r="57" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="4"/>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
-      <c r="E57" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="F57" s="2" t="s">
-        <v>80</v>
-      </c>
-      <c r="G57" s="2"/>
-      <c r="H57" s="2"/>
+      <c r="E57" s="13" t="s">
+        <v>77</v>
+      </c>
+      <c r="F57" s="8" t="s">
+        <v>79</v>
+      </c>
+      <c r="G57" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H57" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="I57" s="4"/>
       <c r="J57" s="4"/>
       <c r="K57" s="4"/>
@@ -3550,21 +3548,21 @@
       <c r="AE57" s="4"/>
       <c r="AF57" s="4"/>
     </row>
-    <row r="58" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A58" s="4"/>
       <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="F58" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F58" s="8" t="s">
-        <v>83</v>
-      </c>
-      <c r="G58" s="8" t="s">
+      <c r="G58" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H58" s="8" t="s">
+      <c r="H58" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I58" s="4"/>
@@ -3592,16 +3590,16 @@
       <c r="AE58" s="4"/>
       <c r="AF58" s="4"/>
     </row>
-    <row r="59" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A59" s="4"/>
       <c r="B59" s="4"/>
       <c r="C59" s="4"/>
       <c r="D59" s="4"/>
       <c r="E59" s="10" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="G59" s="11" t="s">
         <v>9</v>
@@ -3634,19 +3632,19 @@
       <c r="AE59" s="4"/>
       <c r="AF59" s="4"/>
     </row>
-    <row r="60" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A60" s="4"/>
       <c r="B60" s="4"/>
       <c r="C60" s="4"/>
       <c r="D60" s="4"/>
       <c r="E60" s="10" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="F60" s="11" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="G60" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H60" s="11" t="s">
         <v>10</v>
@@ -3676,19 +3674,19 @@
       <c r="AE60" s="4"/>
       <c r="AF60" s="4"/>
     </row>
-    <row r="61" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="4"/>
       <c r="B61" s="4"/>
       <c r="C61" s="4"/>
       <c r="D61" s="4"/>
       <c r="E61" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="F61" s="11" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="G61" s="11" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H61" s="11" t="s">
         <v>10</v>
@@ -3724,7 +3722,7 @@
       <c r="C62" s="4"/>
       <c r="D62" s="4"/>
       <c r="E62" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="F62" s="11" t="s">
         <v>89</v>
@@ -3766,10 +3764,10 @@
       <c r="C63" s="4"/>
       <c r="D63" s="4"/>
       <c r="E63" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="F63" s="11" t="s">
-        <v>93</v>
+        <v>241</v>
       </c>
       <c r="G63" s="11" t="s">
         <v>9</v>
@@ -3807,17 +3805,17 @@
       <c r="B64" s="4"/>
       <c r="C64" s="4"/>
       <c r="D64" s="4"/>
-      <c r="E64" s="10" t="s">
+      <c r="E64" s="13" t="s">
         <v>91</v>
       </c>
-      <c r="F64" s="11" t="s">
-        <v>255</v>
-      </c>
-      <c r="G64" s="11" t="s">
-        <v>9</v>
-      </c>
-      <c r="H64" s="11" t="s">
-        <v>10</v>
+      <c r="F64" s="8" t="s">
+        <v>78</v>
+      </c>
+      <c r="G64" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H64" s="8" t="s">
+        <v>11</v>
       </c>
       <c r="I64" s="4"/>
       <c r="J64" s="4"/>
@@ -3844,58 +3842,58 @@
       <c r="AE64" s="4"/>
       <c r="AF64" s="4"/>
     </row>
-    <row r="65" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="4"/>
-      <c r="B65" s="4"/>
-      <c r="C65" s="4"/>
-      <c r="D65" s="4"/>
-      <c r="E65" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="F65" s="8" t="s">
-        <v>82</v>
-      </c>
-      <c r="G65" s="8" t="s">
+    <row r="65" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A65" s="9"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="9"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="10" t="s">
+        <v>93</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="G65" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H65" s="8" t="s">
+      <c r="H65" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I65" s="4"/>
-      <c r="J65" s="4"/>
-      <c r="K65" s="4"/>
-      <c r="L65" s="4"/>
-      <c r="M65" s="4"/>
-      <c r="N65" s="4"/>
-      <c r="O65" s="4"/>
-      <c r="P65" s="4"/>
-      <c r="Q65" s="4"/>
-      <c r="R65" s="4"/>
-      <c r="S65" s="4"/>
-      <c r="T65" s="4"/>
-      <c r="U65" s="4"/>
-      <c r="V65" s="4"/>
-      <c r="W65" s="4"/>
-      <c r="X65" s="4"/>
-      <c r="Y65" s="4"/>
-      <c r="Z65" s="4"/>
-      <c r="AA65" s="4"/>
-      <c r="AB65" s="4"/>
-      <c r="AC65" s="4"/>
-      <c r="AD65" s="4"/>
-      <c r="AE65" s="4"/>
-      <c r="AF65" s="4"/>
-    </row>
-    <row r="66" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I65" s="9"/>
+      <c r="J65" s="9"/>
+      <c r="K65" s="9"/>
+      <c r="L65" s="9"/>
+      <c r="M65" s="9"/>
+      <c r="N65" s="9"/>
+      <c r="O65" s="9"/>
+      <c r="P65" s="9"/>
+      <c r="Q65" s="9"/>
+      <c r="R65" s="9"/>
+      <c r="S65" s="9"/>
+      <c r="T65" s="9"/>
+      <c r="U65" s="9"/>
+      <c r="V65" s="9"/>
+      <c r="W65" s="9"/>
+      <c r="X65" s="9"/>
+      <c r="Y65" s="9"/>
+      <c r="Z65" s="9"/>
+      <c r="AA65" s="9"/>
+      <c r="AB65" s="9"/>
+      <c r="AC65" s="9"/>
+      <c r="AD65" s="9"/>
+      <c r="AE65" s="9"/>
+      <c r="AF65" s="9"/>
+    </row>
+    <row r="66" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A66" s="9"/>
       <c r="B66" s="9"/>
       <c r="C66" s="9"/>
       <c r="D66" s="9"/>
       <c r="E66" s="10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="F66" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G66" s="11" t="s">
         <v>16</v>
@@ -3928,184 +3926,184 @@
       <c r="AE66" s="9"/>
       <c r="AF66" s="9"/>
     </row>
-    <row r="67" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A67" s="9"/>
-      <c r="B67" s="9"/>
-      <c r="C67" s="9"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="10" t="s">
+    <row r="67" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="4"/>
+      <c r="B67" s="4"/>
+      <c r="C67" s="4"/>
+      <c r="D67" s="4"/>
+      <c r="E67" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="F67" s="8" t="s">
+        <v>98</v>
+      </c>
+      <c r="G67" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H67" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I67" s="4"/>
+      <c r="J67" s="4"/>
+      <c r="K67" s="4"/>
+      <c r="L67" s="4"/>
+      <c r="M67" s="4"/>
+      <c r="N67" s="4"/>
+      <c r="O67" s="4"/>
+      <c r="P67" s="4"/>
+      <c r="Q67" s="4"/>
+      <c r="R67" s="4"/>
+      <c r="S67" s="4"/>
+      <c r="T67" s="4"/>
+      <c r="U67" s="4"/>
+      <c r="V67" s="4"/>
+      <c r="W67" s="4"/>
+      <c r="X67" s="4"/>
+      <c r="Y67" s="4"/>
+      <c r="Z67" s="4"/>
+      <c r="AA67" s="4"/>
+      <c r="AB67" s="4"/>
+      <c r="AC67" s="4"/>
+      <c r="AD67" s="4"/>
+      <c r="AE67" s="4"/>
+      <c r="AF67" s="4"/>
+    </row>
+    <row r="68" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="9"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="9"/>
+      <c r="D68" s="9"/>
+      <c r="E68" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="F68" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="F67" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="G67" s="11" t="s">
+      <c r="G68" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H67" s="11" t="s">
+      <c r="H68" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I67" s="9"/>
-      <c r="J67" s="9"/>
-      <c r="K67" s="9"/>
-      <c r="L67" s="9"/>
-      <c r="M67" s="9"/>
-      <c r="N67" s="9"/>
-      <c r="O67" s="9"/>
-      <c r="P67" s="9"/>
-      <c r="Q67" s="9"/>
-      <c r="R67" s="9"/>
-      <c r="S67" s="9"/>
-      <c r="T67" s="9"/>
-      <c r="U67" s="9"/>
-      <c r="V67" s="9"/>
-      <c r="W67" s="9"/>
-      <c r="X67" s="9"/>
-      <c r="Y67" s="9"/>
-      <c r="Z67" s="9"/>
-      <c r="AA67" s="9"/>
-      <c r="AB67" s="9"/>
-      <c r="AC67" s="9"/>
-      <c r="AD67" s="9"/>
-      <c r="AE67" s="9"/>
-      <c r="AF67" s="9"/>
-    </row>
-    <row r="68" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A68" s="4"/>
-      <c r="B68" s="4"/>
-      <c r="C68" s="4"/>
-      <c r="D68" s="4"/>
-      <c r="E68" s="13" t="s">
+      <c r="I68" s="9"/>
+      <c r="J68" s="9"/>
+      <c r="K68" s="9"/>
+      <c r="L68" s="9"/>
+      <c r="M68" s="9"/>
+      <c r="N68" s="9"/>
+      <c r="O68" s="9"/>
+      <c r="P68" s="9"/>
+      <c r="Q68" s="9"/>
+      <c r="R68" s="9"/>
+      <c r="S68" s="9"/>
+      <c r="T68" s="9"/>
+      <c r="U68" s="9"/>
+      <c r="V68" s="9"/>
+      <c r="W68" s="9"/>
+      <c r="X68" s="9"/>
+      <c r="Y68" s="9"/>
+      <c r="Z68" s="9"/>
+      <c r="AA68" s="9"/>
+      <c r="AB68" s="9"/>
+      <c r="AC68" s="9"/>
+      <c r="AD68" s="9"/>
+      <c r="AE68" s="9"/>
+      <c r="AF68" s="9"/>
+    </row>
+    <row r="69" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A69" s="4"/>
+      <c r="B69" s="4"/>
+      <c r="C69" s="4"/>
+      <c r="D69" s="4"/>
+      <c r="E69" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="F68" s="8" t="s">
+      <c r="F69" s="8" t="s">
+        <v>101</v>
+      </c>
+      <c r="G69" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H69" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I69" s="4"/>
+      <c r="J69" s="4"/>
+      <c r="K69" s="4"/>
+      <c r="L69" s="4"/>
+      <c r="M69" s="4"/>
+      <c r="N69" s="4"/>
+      <c r="O69" s="4"/>
+      <c r="P69" s="4"/>
+      <c r="Q69" s="4"/>
+      <c r="R69" s="4"/>
+      <c r="S69" s="4"/>
+      <c r="T69" s="4"/>
+      <c r="U69" s="4"/>
+      <c r="V69" s="4"/>
+      <c r="W69" s="4"/>
+      <c r="X69" s="4"/>
+      <c r="Y69" s="4"/>
+      <c r="Z69" s="4"/>
+      <c r="AA69" s="4"/>
+      <c r="AB69" s="4"/>
+      <c r="AC69" s="4"/>
+      <c r="AD69" s="4"/>
+      <c r="AE69" s="4"/>
+      <c r="AF69" s="4"/>
+    </row>
+    <row r="70" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A70" s="9"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="9"/>
+      <c r="D70" s="9"/>
+      <c r="E70" s="10" t="s">
         <v>102</v>
       </c>
-      <c r="G68" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H68" s="8" t="s">
-        <v>11</v>
-      </c>
-      <c r="I68" s="4"/>
-      <c r="J68" s="4"/>
-      <c r="K68" s="4"/>
-      <c r="L68" s="4"/>
-      <c r="M68" s="4"/>
-      <c r="N68" s="4"/>
-      <c r="O68" s="4"/>
-      <c r="P68" s="4"/>
-      <c r="Q68" s="4"/>
-      <c r="R68" s="4"/>
-      <c r="S68" s="4"/>
-      <c r="T68" s="4"/>
-      <c r="U68" s="4"/>
-      <c r="V68" s="4"/>
-      <c r="W68" s="4"/>
-      <c r="X68" s="4"/>
-      <c r="Y68" s="4"/>
-      <c r="Z68" s="4"/>
-      <c r="AA68" s="4"/>
-      <c r="AB68" s="4"/>
-      <c r="AC68" s="4"/>
-      <c r="AD68" s="4"/>
-      <c r="AE68" s="4"/>
-      <c r="AF68" s="4"/>
-    </row>
-    <row r="69" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="9"/>
-      <c r="B69" s="9"/>
-      <c r="C69" s="9"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="10" t="s">
-        <v>101</v>
-      </c>
-      <c r="F69" s="11" t="s">
-        <v>103</v>
-      </c>
-      <c r="G69" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H69" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I69" s="9"/>
-      <c r="J69" s="9"/>
-      <c r="K69" s="9"/>
-      <c r="L69" s="9"/>
-      <c r="M69" s="9"/>
-      <c r="N69" s="9"/>
-      <c r="O69" s="9"/>
-      <c r="P69" s="9"/>
-      <c r="Q69" s="9"/>
-      <c r="R69" s="9"/>
-      <c r="S69" s="9"/>
-      <c r="T69" s="9"/>
-      <c r="U69" s="9"/>
-      <c r="V69" s="9"/>
-      <c r="W69" s="9"/>
-      <c r="X69" s="9"/>
-      <c r="Y69" s="9"/>
-      <c r="Z69" s="9"/>
-      <c r="AA69" s="9"/>
-      <c r="AB69" s="9"/>
-      <c r="AC69" s="9"/>
-      <c r="AD69" s="9"/>
-      <c r="AE69" s="9"/>
-      <c r="AF69" s="9"/>
-    </row>
-    <row r="70" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A70" s="4"/>
-      <c r="B70" s="4"/>
-      <c r="C70" s="4"/>
-      <c r="D70" s="4"/>
-      <c r="E70" s="13" t="s">
+      <c r="F70" s="11" t="s">
         <v>104</v>
       </c>
-      <c r="F70" s="8" t="s">
-        <v>105</v>
-      </c>
-      <c r="G70" s="8" t="s">
+      <c r="G70" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H70" s="8" t="s">
+      <c r="H70" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I70" s="4"/>
-      <c r="J70" s="4"/>
-      <c r="K70" s="4"/>
-      <c r="L70" s="4"/>
-      <c r="M70" s="4"/>
-      <c r="N70" s="4"/>
-      <c r="O70" s="4"/>
-      <c r="P70" s="4"/>
-      <c r="Q70" s="4"/>
-      <c r="R70" s="4"/>
-      <c r="S70" s="4"/>
-      <c r="T70" s="4"/>
-      <c r="U70" s="4"/>
-      <c r="V70" s="4"/>
-      <c r="W70" s="4"/>
-      <c r="X70" s="4"/>
-      <c r="Y70" s="4"/>
-      <c r="Z70" s="4"/>
-      <c r="AA70" s="4"/>
-      <c r="AB70" s="4"/>
-      <c r="AC70" s="4"/>
-      <c r="AD70" s="4"/>
-      <c r="AE70" s="4"/>
-      <c r="AF70" s="4"/>
-    </row>
-    <row r="71" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I70" s="9"/>
+      <c r="J70" s="9"/>
+      <c r="K70" s="9"/>
+      <c r="L70" s="9"/>
+      <c r="M70" s="9"/>
+      <c r="N70" s="9"/>
+      <c r="O70" s="9"/>
+      <c r="P70" s="9"/>
+      <c r="Q70" s="9"/>
+      <c r="R70" s="9"/>
+      <c r="S70" s="9"/>
+      <c r="T70" s="9"/>
+      <c r="U70" s="9"/>
+      <c r="V70" s="9"/>
+      <c r="W70" s="9"/>
+      <c r="X70" s="9"/>
+      <c r="Y70" s="9"/>
+      <c r="Z70" s="9"/>
+      <c r="AA70" s="9"/>
+      <c r="AB70" s="9"/>
+      <c r="AC70" s="9"/>
+      <c r="AD70" s="9"/>
+      <c r="AE70" s="9"/>
+      <c r="AF70" s="9"/>
+    </row>
+    <row r="71" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="9"/>
       <c r="B71" s="9"/>
       <c r="C71" s="9"/>
       <c r="D71" s="9"/>
       <c r="E71" s="10" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="F71" s="11" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="G71" s="11" t="s">
         <v>9</v>
@@ -4138,89 +4136,89 @@
       <c r="AE71" s="9"/>
       <c r="AF71" s="9"/>
     </row>
-    <row r="72" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="9"/>
-      <c r="B72" s="9"/>
-      <c r="C72" s="9"/>
-      <c r="D72" s="9"/>
-      <c r="E72" s="10" t="s">
+    <row r="72" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="4"/>
+      <c r="B72" s="4"/>
+      <c r="C72" s="4"/>
+      <c r="D72" s="4"/>
+      <c r="E72" s="13" t="s">
+        <v>106</v>
+      </c>
+      <c r="F72" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="G72" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H72" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I72" s="4"/>
+      <c r="J72" s="4"/>
+      <c r="K72" s="4"/>
+      <c r="L72" s="4"/>
+      <c r="M72" s="4"/>
+      <c r="N72" s="4"/>
+      <c r="O72" s="4"/>
+      <c r="P72" s="4"/>
+      <c r="Q72" s="4"/>
+      <c r="R72" s="4"/>
+      <c r="S72" s="4"/>
+      <c r="T72" s="4"/>
+      <c r="U72" s="4"/>
+      <c r="V72" s="4"/>
+      <c r="W72" s="4"/>
+      <c r="X72" s="4"/>
+      <c r="Y72" s="4"/>
+      <c r="Z72" s="4"/>
+      <c r="AA72" s="4"/>
+      <c r="AB72" s="4"/>
+      <c r="AC72" s="4"/>
+      <c r="AD72" s="4"/>
+      <c r="AE72" s="4"/>
+      <c r="AF72" s="4"/>
+    </row>
+    <row r="73" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="9"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="9"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="10" t="s">
         <v>107</v>
       </c>
-      <c r="F72" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="G72" s="11" t="s">
+      <c r="F73" s="11" t="s">
+        <v>110</v>
+      </c>
+      <c r="G73" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H72" s="11" t="s">
+      <c r="H73" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I72" s="9"/>
-      <c r="J72" s="9"/>
-      <c r="K72" s="9"/>
-      <c r="L72" s="9"/>
-      <c r="M72" s="9"/>
-      <c r="N72" s="9"/>
-      <c r="O72" s="9"/>
-      <c r="P72" s="9"/>
-      <c r="Q72" s="9"/>
-      <c r="R72" s="9"/>
-      <c r="S72" s="9"/>
-      <c r="T72" s="9"/>
-      <c r="U72" s="9"/>
-      <c r="V72" s="9"/>
-      <c r="W72" s="9"/>
-      <c r="X72" s="9"/>
-      <c r="Y72" s="9"/>
-      <c r="Z72" s="9"/>
-      <c r="AA72" s="9"/>
-      <c r="AB72" s="9"/>
-      <c r="AC72" s="9"/>
-      <c r="AD72" s="9"/>
-      <c r="AE72" s="9"/>
-      <c r="AF72" s="9"/>
-    </row>
-    <row r="73" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="4"/>
-      <c r="B73" s="4"/>
-      <c r="C73" s="4"/>
-      <c r="D73" s="4"/>
-      <c r="E73" s="13" t="s">
-        <v>110</v>
-      </c>
-      <c r="F73" s="8" t="s">
-        <v>113</v>
-      </c>
-      <c r="G73" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H73" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I73" s="4"/>
-      <c r="J73" s="4"/>
-      <c r="K73" s="4"/>
-      <c r="L73" s="4"/>
-      <c r="M73" s="4"/>
-      <c r="N73" s="4"/>
-      <c r="O73" s="4"/>
-      <c r="P73" s="4"/>
-      <c r="Q73" s="4"/>
-      <c r="R73" s="4"/>
-      <c r="S73" s="4"/>
-      <c r="T73" s="4"/>
-      <c r="U73" s="4"/>
-      <c r="V73" s="4"/>
-      <c r="W73" s="4"/>
-      <c r="X73" s="4"/>
-      <c r="Y73" s="4"/>
-      <c r="Z73" s="4"/>
-      <c r="AA73" s="4"/>
-      <c r="AB73" s="4"/>
-      <c r="AC73" s="4"/>
-      <c r="AD73" s="4"/>
-      <c r="AE73" s="4"/>
-      <c r="AF73" s="4"/>
+      <c r="I73" s="9"/>
+      <c r="J73" s="9"/>
+      <c r="K73" s="9"/>
+      <c r="L73" s="9"/>
+      <c r="M73" s="9"/>
+      <c r="N73" s="9"/>
+      <c r="O73" s="9"/>
+      <c r="P73" s="9"/>
+      <c r="Q73" s="9"/>
+      <c r="R73" s="9"/>
+      <c r="S73" s="9"/>
+      <c r="T73" s="9"/>
+      <c r="U73" s="9"/>
+      <c r="V73" s="9"/>
+      <c r="W73" s="9"/>
+      <c r="X73" s="9"/>
+      <c r="Y73" s="9"/>
+      <c r="Z73" s="9"/>
+      <c r="AA73" s="9"/>
+      <c r="AB73" s="9"/>
+      <c r="AC73" s="9"/>
+      <c r="AD73" s="9"/>
+      <c r="AE73" s="9"/>
+      <c r="AF73" s="9"/>
     </row>
     <row r="74" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="9"/>
@@ -4228,10 +4226,10 @@
       <c r="C74" s="9"/>
       <c r="D74" s="9"/>
       <c r="E74" s="10" t="s">
+        <v>108</v>
+      </c>
+      <c r="F74" s="11" t="s">
         <v>111</v>
-      </c>
-      <c r="F74" s="11" t="s">
-        <v>114</v>
       </c>
       <c r="G74" s="11" t="s">
         <v>9</v>
@@ -4264,16 +4262,16 @@
       <c r="AE74" s="9"/>
       <c r="AF74" s="9"/>
     </row>
-    <row r="75" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A75" s="9"/>
       <c r="B75" s="9"/>
       <c r="C75" s="9"/>
       <c r="D75" s="9"/>
       <c r="E75" s="10" t="s">
-        <v>112</v>
+        <v>124</v>
       </c>
       <c r="F75" s="11" t="s">
-        <v>115</v>
+        <v>123</v>
       </c>
       <c r="G75" s="11" t="s">
         <v>9</v>
@@ -4306,16 +4304,16 @@
       <c r="AE75" s="9"/>
       <c r="AF75" s="9"/>
     </row>
-    <row r="76" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A76" s="9"/>
       <c r="B76" s="9"/>
       <c r="C76" s="9"/>
       <c r="D76" s="9"/>
       <c r="E76" s="10" t="s">
-        <v>128</v>
+        <v>125</v>
       </c>
       <c r="F76" s="11" t="s">
-        <v>127</v>
+        <v>122</v>
       </c>
       <c r="G76" s="11" t="s">
         <v>9</v>
@@ -4348,63 +4346,63 @@
       <c r="AE76" s="9"/>
       <c r="AF76" s="9"/>
     </row>
-    <row r="77" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A77" s="9"/>
-      <c r="B77" s="9"/>
-      <c r="C77" s="9"/>
-      <c r="D77" s="9"/>
-      <c r="E77" s="10" t="s">
-        <v>129</v>
-      </c>
-      <c r="F77" s="11" t="s">
-        <v>126</v>
-      </c>
-      <c r="G77" s="11" t="s">
+    <row r="77" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A77" s="4"/>
+      <c r="B77" s="4"/>
+      <c r="C77" s="4"/>
+      <c r="D77" s="4"/>
+      <c r="E77" s="13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="G77" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H77" s="11" t="s">
+      <c r="H77" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I77" s="9"/>
-      <c r="J77" s="9"/>
-      <c r="K77" s="9"/>
-      <c r="L77" s="9"/>
-      <c r="M77" s="9"/>
-      <c r="N77" s="9"/>
-      <c r="O77" s="9"/>
-      <c r="P77" s="9"/>
-      <c r="Q77" s="9"/>
-      <c r="R77" s="9"/>
-      <c r="S77" s="9"/>
-      <c r="T77" s="9"/>
-      <c r="U77" s="9"/>
-      <c r="V77" s="9"/>
-      <c r="W77" s="9"/>
-      <c r="X77" s="9"/>
-      <c r="Y77" s="9"/>
-      <c r="Z77" s="9"/>
-      <c r="AA77" s="9"/>
-      <c r="AB77" s="9"/>
-      <c r="AC77" s="9"/>
-      <c r="AD77" s="9"/>
-      <c r="AE77" s="9"/>
-      <c r="AF77" s="9"/>
-    </row>
-    <row r="78" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I77" s="4"/>
+      <c r="J77" s="4"/>
+      <c r="K77" s="4"/>
+      <c r="L77" s="4"/>
+      <c r="M77" s="4"/>
+      <c r="N77" s="4"/>
+      <c r="O77" s="4"/>
+      <c r="P77" s="4"/>
+      <c r="Q77" s="4"/>
+      <c r="R77" s="4"/>
+      <c r="S77" s="4"/>
+      <c r="T77" s="4"/>
+      <c r="U77" s="4"/>
+      <c r="V77" s="4"/>
+      <c r="W77" s="4"/>
+      <c r="X77" s="4"/>
+      <c r="Y77" s="4"/>
+      <c r="Z77" s="4"/>
+      <c r="AA77" s="4"/>
+      <c r="AB77" s="4"/>
+      <c r="AC77" s="4"/>
+      <c r="AD77" s="4"/>
+      <c r="AE77" s="4"/>
+      <c r="AF77" s="4"/>
+    </row>
+    <row r="78" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A78" s="4"/>
       <c r="B78" s="4"/>
       <c r="C78" s="4"/>
       <c r="D78" s="4"/>
-      <c r="E78" s="13" t="s">
-        <v>116</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>117</v>
-      </c>
-      <c r="G78" s="8" t="s">
+      <c r="E78" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="F78" s="11" t="s">
+        <v>115</v>
+      </c>
+      <c r="G78" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H78" s="8" t="s">
+      <c r="H78" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I78" s="4"/>
@@ -4438,10 +4436,10 @@
       <c r="C79" s="4"/>
       <c r="D79" s="4"/>
       <c r="E79" s="10" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="F79" s="11" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="G79" s="11" t="s">
         <v>9</v>
@@ -4480,10 +4478,10 @@
       <c r="C80" s="4"/>
       <c r="D80" s="4"/>
       <c r="E80" s="10" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="F80" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G80" s="11" t="s">
         <v>9</v>
@@ -4516,16 +4514,16 @@
       <c r="AE80" s="4"/>
       <c r="AF80" s="4"/>
     </row>
-    <row r="81" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A81" s="4"/>
       <c r="B81" s="4"/>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
       <c r="E81" s="10" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="F81" s="11" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G81" s="11" t="s">
         <v>9</v>
@@ -4564,13 +4562,13 @@
       <c r="C82" s="4"/>
       <c r="D82" s="4"/>
       <c r="E82" s="10" t="s">
-        <v>124</v>
+        <v>213</v>
       </c>
       <c r="F82" s="11" t="s">
-        <v>125</v>
+        <v>212</v>
       </c>
       <c r="G82" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H82" s="11" t="s">
         <v>10</v>
@@ -4605,18 +4603,14 @@
       <c r="B83" s="4"/>
       <c r="C83" s="4"/>
       <c r="D83" s="4"/>
-      <c r="E83" s="10" t="s">
-        <v>220</v>
-      </c>
-      <c r="F83" s="11" t="s">
-        <v>219</v>
-      </c>
-      <c r="G83" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H83" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="E83" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="F83" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="G83" s="2"/>
+      <c r="H83" s="2"/>
       <c r="I83" s="4"/>
       <c r="J83" s="4"/>
       <c r="K83" s="4"/>
@@ -4647,14 +4641,18 @@
       <c r="B84" s="4"/>
       <c r="C84" s="4"/>
       <c r="D84" s="4"/>
-      <c r="E84" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="F84" s="2" t="s">
+      <c r="E84" s="13" t="s">
+        <v>128</v>
+      </c>
+      <c r="F84" s="8" t="s">
         <v>131</v>
       </c>
-      <c r="G84" s="2"/>
-      <c r="H84" s="2"/>
+      <c r="G84" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H84" s="8" t="s">
+        <v>11</v>
+      </c>
       <c r="I84" s="4"/>
       <c r="J84" s="4"/>
       <c r="K84" s="4"/>
@@ -4685,16 +4683,16 @@
       <c r="B85" s="4"/>
       <c r="C85" s="4"/>
       <c r="D85" s="4"/>
-      <c r="E85" s="13" t="s">
+      <c r="E85" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="F85" s="11" t="s">
         <v>132</v>
       </c>
-      <c r="F85" s="8" t="s">
-        <v>135</v>
-      </c>
-      <c r="G85" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="H85" s="8" t="s">
+      <c r="G85" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H85" s="11" t="s">
         <v>11</v>
       </c>
       <c r="I85" s="4"/>
@@ -4722,131 +4720,131 @@
       <c r="AE85" s="4"/>
       <c r="AF85" s="4"/>
     </row>
-    <row r="86" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A86" s="4"/>
-      <c r="B86" s="4"/>
-      <c r="C86" s="4"/>
-      <c r="D86" s="4"/>
+    <row r="86" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A86" s="9"/>
+      <c r="B86" s="9"/>
+      <c r="C86" s="9"/>
+      <c r="D86" s="9"/>
       <c r="E86" s="10" t="s">
         <v>133</v>
       </c>
       <c r="F86" s="11" t="s">
-        <v>136</v>
+        <v>130</v>
       </c>
       <c r="G86" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H86" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="I86" s="4"/>
-      <c r="J86" s="4"/>
-      <c r="K86" s="4"/>
-      <c r="L86" s="4"/>
-      <c r="M86" s="4"/>
-      <c r="N86" s="4"/>
-      <c r="O86" s="4"/>
-      <c r="P86" s="4"/>
-      <c r="Q86" s="4"/>
-      <c r="R86" s="4"/>
-      <c r="S86" s="4"/>
-      <c r="T86" s="4"/>
-      <c r="U86" s="4"/>
-      <c r="V86" s="4"/>
-      <c r="W86" s="4"/>
-      <c r="X86" s="4"/>
-      <c r="Y86" s="4"/>
-      <c r="Z86" s="4"/>
-      <c r="AA86" s="4"/>
-      <c r="AB86" s="4"/>
-      <c r="AC86" s="4"/>
-      <c r="AD86" s="4"/>
-      <c r="AE86" s="4"/>
-      <c r="AF86" s="4"/>
-    </row>
-    <row r="87" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A87" s="9"/>
-      <c r="B87" s="9"/>
-      <c r="C87" s="9"/>
-      <c r="D87" s="9"/>
-      <c r="E87" s="10" t="s">
-        <v>137</v>
-      </c>
-      <c r="F87" s="11" t="s">
+      <c r="I86" s="9"/>
+      <c r="J86" s="9"/>
+      <c r="K86" s="9"/>
+      <c r="L86" s="9"/>
+      <c r="M86" s="9"/>
+      <c r="N86" s="9"/>
+      <c r="O86" s="9"/>
+      <c r="P86" s="9"/>
+      <c r="Q86" s="9"/>
+      <c r="R86" s="9"/>
+      <c r="S86" s="9"/>
+      <c r="T86" s="9"/>
+      <c r="U86" s="9"/>
+      <c r="V86" s="9"/>
+      <c r="W86" s="9"/>
+      <c r="X86" s="9"/>
+      <c r="Y86" s="9"/>
+      <c r="Z86" s="9"/>
+      <c r="AA86" s="9"/>
+      <c r="AB86" s="9"/>
+      <c r="AC86" s="9"/>
+      <c r="AD86" s="9"/>
+      <c r="AE86" s="9"/>
+      <c r="AF86" s="9"/>
+    </row>
+    <row r="87" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A87" s="4"/>
+      <c r="B87" s="4"/>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4"/>
+      <c r="E87" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="G87" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H87" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I87" s="9"/>
-      <c r="J87" s="9"/>
-      <c r="K87" s="9"/>
-      <c r="L87" s="9"/>
-      <c r="M87" s="9"/>
-      <c r="N87" s="9"/>
-      <c r="O87" s="9"/>
-      <c r="P87" s="9"/>
-      <c r="Q87" s="9"/>
-      <c r="R87" s="9"/>
-      <c r="S87" s="9"/>
-      <c r="T87" s="9"/>
-      <c r="U87" s="9"/>
-      <c r="V87" s="9"/>
-      <c r="W87" s="9"/>
-      <c r="X87" s="9"/>
-      <c r="Y87" s="9"/>
-      <c r="Z87" s="9"/>
-      <c r="AA87" s="9"/>
-      <c r="AB87" s="9"/>
-      <c r="AC87" s="9"/>
-      <c r="AD87" s="9"/>
-      <c r="AE87" s="9"/>
-      <c r="AF87" s="9"/>
-    </row>
-    <row r="88" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A88" s="4"/>
-      <c r="B88" s="4"/>
-      <c r="C88" s="4"/>
-      <c r="D88" s="4"/>
-      <c r="E88" s="13" t="s">
-        <v>138</v>
-      </c>
-      <c r="F88" s="8" t="s">
+      <c r="F87" s="8" t="s">
+        <v>135</v>
+      </c>
+      <c r="G87" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H87" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I87" s="4"/>
+      <c r="J87" s="4"/>
+      <c r="K87" s="4"/>
+      <c r="L87" s="4"/>
+      <c r="M87" s="4"/>
+      <c r="N87" s="4"/>
+      <c r="O87" s="4"/>
+      <c r="P87" s="4"/>
+      <c r="Q87" s="4"/>
+      <c r="R87" s="4"/>
+      <c r="S87" s="4"/>
+      <c r="T87" s="4"/>
+      <c r="U87" s="4"/>
+      <c r="V87" s="4"/>
+      <c r="W87" s="4"/>
+      <c r="X87" s="4"/>
+      <c r="Y87" s="4"/>
+      <c r="Z87" s="4"/>
+      <c r="AA87" s="4"/>
+      <c r="AB87" s="4"/>
+      <c r="AC87" s="4"/>
+      <c r="AD87" s="4"/>
+      <c r="AE87" s="4"/>
+      <c r="AF87" s="4"/>
+    </row>
+    <row r="88" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="9"/>
+      <c r="B88" s="9"/>
+      <c r="C88" s="9"/>
+      <c r="D88" s="9"/>
+      <c r="E88" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="F88" s="11" t="s">
         <v>139</v>
       </c>
-      <c r="G88" s="8" t="s">
+      <c r="G88" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H88" s="8" t="s">
+      <c r="H88" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I88" s="4"/>
-      <c r="J88" s="4"/>
-      <c r="K88" s="4"/>
-      <c r="L88" s="4"/>
-      <c r="M88" s="4"/>
-      <c r="N88" s="4"/>
-      <c r="O88" s="4"/>
-      <c r="P88" s="4"/>
-      <c r="Q88" s="4"/>
-      <c r="R88" s="4"/>
-      <c r="S88" s="4"/>
-      <c r="T88" s="4"/>
-      <c r="U88" s="4"/>
-      <c r="V88" s="4"/>
-      <c r="W88" s="4"/>
-      <c r="X88" s="4"/>
-      <c r="Y88" s="4"/>
-      <c r="Z88" s="4"/>
-      <c r="AA88" s="4"/>
-      <c r="AB88" s="4"/>
-      <c r="AC88" s="4"/>
-      <c r="AD88" s="4"/>
-      <c r="AE88" s="4"/>
-      <c r="AF88" s="4"/>
+      <c r="I88" s="9"/>
+      <c r="J88" s="9"/>
+      <c r="K88" s="9"/>
+      <c r="L88" s="9"/>
+      <c r="M88" s="9"/>
+      <c r="N88" s="9"/>
+      <c r="O88" s="9"/>
+      <c r="P88" s="9"/>
+      <c r="Q88" s="9"/>
+      <c r="R88" s="9"/>
+      <c r="S88" s="9"/>
+      <c r="T88" s="9"/>
+      <c r="U88" s="9"/>
+      <c r="V88" s="9"/>
+      <c r="W88" s="9"/>
+      <c r="X88" s="9"/>
+      <c r="Y88" s="9"/>
+      <c r="Z88" s="9"/>
+      <c r="AA88" s="9"/>
+      <c r="AB88" s="9"/>
+      <c r="AC88" s="9"/>
+      <c r="AD88" s="9"/>
+      <c r="AE88" s="9"/>
+      <c r="AF88" s="9"/>
     </row>
     <row r="89" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A89" s="9"/>
@@ -4854,10 +4852,10 @@
       <c r="C89" s="9"/>
       <c r="D89" s="9"/>
       <c r="E89" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="F89" s="11" t="s">
         <v>140</v>
-      </c>
-      <c r="F89" s="11" t="s">
-        <v>143</v>
       </c>
       <c r="G89" s="11" t="s">
         <v>9</v>
@@ -4896,13 +4894,13 @@
       <c r="C90" s="9"/>
       <c r="D90" s="9"/>
       <c r="E90" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="F90" s="11" t="s">
         <v>141</v>
       </c>
-      <c r="F90" s="11" t="s">
-        <v>144</v>
-      </c>
       <c r="G90" s="11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H90" s="11" t="s">
         <v>10</v>
@@ -4932,100 +4930,100 @@
       <c r="AE90" s="9"/>
       <c r="AF90" s="9"/>
     </row>
-    <row r="91" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A91" s="9"/>
-      <c r="B91" s="9"/>
-      <c r="C91" s="9"/>
-      <c r="D91" s="9"/>
-      <c r="E91" s="10" t="s">
+    <row r="91" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A91" s="4"/>
+      <c r="B91" s="4"/>
+      <c r="C91" s="4"/>
+      <c r="D91" s="4"/>
+      <c r="E91" s="13" t="s">
+        <v>143</v>
+      </c>
+      <c r="F91" s="8" t="s">
         <v>142</v>
       </c>
-      <c r="F91" s="11" t="s">
+      <c r="G91" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H91" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I91" s="4"/>
+      <c r="J91" s="4"/>
+      <c r="K91" s="4"/>
+      <c r="L91" s="4"/>
+      <c r="M91" s="4"/>
+      <c r="N91" s="4"/>
+      <c r="O91" s="4"/>
+      <c r="P91" s="4"/>
+      <c r="Q91" s="4"/>
+      <c r="R91" s="4"/>
+      <c r="S91" s="4"/>
+      <c r="T91" s="4"/>
+      <c r="U91" s="4"/>
+      <c r="V91" s="4"/>
+      <c r="W91" s="4"/>
+      <c r="X91" s="4"/>
+      <c r="Y91" s="4"/>
+      <c r="Z91" s="4"/>
+      <c r="AA91" s="4"/>
+      <c r="AB91" s="4"/>
+      <c r="AC91" s="4"/>
+      <c r="AD91" s="4"/>
+      <c r="AE91" s="4"/>
+      <c r="AF91" s="4"/>
+    </row>
+    <row r="92" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A92" s="9"/>
+      <c r="B92" s="9"/>
+      <c r="C92" s="9"/>
+      <c r="D92" s="9"/>
+      <c r="E92" s="10" t="s">
         <v>145</v>
       </c>
-      <c r="G91" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="H91" s="11" t="s">
+      <c r="F92" s="11" t="s">
+        <v>144</v>
+      </c>
+      <c r="G92" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="H92" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I91" s="9"/>
-      <c r="J91" s="9"/>
-      <c r="K91" s="9"/>
-      <c r="L91" s="9"/>
-      <c r="M91" s="9"/>
-      <c r="N91" s="9"/>
-      <c r="O91" s="9"/>
-      <c r="P91" s="9"/>
-      <c r="Q91" s="9"/>
-      <c r="R91" s="9"/>
-      <c r="S91" s="9"/>
-      <c r="T91" s="9"/>
-      <c r="U91" s="9"/>
-      <c r="V91" s="9"/>
-      <c r="W91" s="9"/>
-      <c r="X91" s="9"/>
-      <c r="Y91" s="9"/>
-      <c r="Z91" s="9"/>
-      <c r="AA91" s="9"/>
-      <c r="AB91" s="9"/>
-      <c r="AC91" s="9"/>
-      <c r="AD91" s="9"/>
-      <c r="AE91" s="9"/>
-      <c r="AF91" s="9"/>
-    </row>
-    <row r="92" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A92" s="4"/>
-      <c r="B92" s="4"/>
-      <c r="C92" s="4"/>
-      <c r="D92" s="4"/>
-      <c r="E92" s="13" t="s">
-        <v>147</v>
-      </c>
-      <c r="F92" s="8" t="s">
-        <v>146</v>
-      </c>
-      <c r="G92" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H92" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I92" s="4"/>
-      <c r="J92" s="4"/>
-      <c r="K92" s="4"/>
-      <c r="L92" s="4"/>
-      <c r="M92" s="4"/>
-      <c r="N92" s="4"/>
-      <c r="O92" s="4"/>
-      <c r="P92" s="4"/>
-      <c r="Q92" s="4"/>
-      <c r="R92" s="4"/>
-      <c r="S92" s="4"/>
-      <c r="T92" s="4"/>
-      <c r="U92" s="4"/>
-      <c r="V92" s="4"/>
-      <c r="W92" s="4"/>
-      <c r="X92" s="4"/>
-      <c r="Y92" s="4"/>
-      <c r="Z92" s="4"/>
-      <c r="AA92" s="4"/>
-      <c r="AB92" s="4"/>
-      <c r="AC92" s="4"/>
-      <c r="AD92" s="4"/>
-      <c r="AE92" s="4"/>
-      <c r="AF92" s="4"/>
-    </row>
-    <row r="93" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I92" s="9"/>
+      <c r="J92" s="9"/>
+      <c r="K92" s="9"/>
+      <c r="L92" s="9"/>
+      <c r="M92" s="9"/>
+      <c r="N92" s="9"/>
+      <c r="O92" s="9"/>
+      <c r="P92" s="9"/>
+      <c r="Q92" s="9"/>
+      <c r="R92" s="9"/>
+      <c r="S92" s="9"/>
+      <c r="T92" s="9"/>
+      <c r="U92" s="9"/>
+      <c r="V92" s="9"/>
+      <c r="W92" s="9"/>
+      <c r="X92" s="9"/>
+      <c r="Y92" s="9"/>
+      <c r="Z92" s="9"/>
+      <c r="AA92" s="9"/>
+      <c r="AB92" s="9"/>
+      <c r="AC92" s="9"/>
+      <c r="AD92" s="9"/>
+      <c r="AE92" s="9"/>
+      <c r="AF92" s="9"/>
+    </row>
+    <row r="93" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A93" s="9"/>
       <c r="B93" s="9"/>
       <c r="C93" s="9"/>
       <c r="D93" s="9"/>
       <c r="E93" s="10" t="s">
+        <v>148</v>
+      </c>
+      <c r="F93" s="11" t="s">
         <v>149</v>
-      </c>
-      <c r="F93" s="11" t="s">
-        <v>148</v>
       </c>
       <c r="G93" s="11" t="s">
         <v>9</v>
@@ -5058,19 +5056,19 @@
       <c r="AE93" s="9"/>
       <c r="AF93" s="9"/>
     </row>
-    <row r="94" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A94" s="9"/>
       <c r="B94" s="9"/>
       <c r="C94" s="9"/>
       <c r="D94" s="9"/>
       <c r="E94" s="10" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="F94" s="11" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="G94" s="11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H94" s="11" t="s">
         <v>10</v>
@@ -5100,7 +5098,7 @@
       <c r="AE94" s="9"/>
       <c r="AF94" s="9"/>
     </row>
-    <row r="95" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A95" s="9"/>
       <c r="B95" s="9"/>
       <c r="C95" s="9"/>
@@ -5112,7 +5110,7 @@
         <v>155</v>
       </c>
       <c r="G95" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H95" s="11" t="s">
         <v>10</v>
@@ -5148,10 +5146,10 @@
       <c r="C96" s="9"/>
       <c r="D96" s="9"/>
       <c r="E96" s="10" t="s">
-        <v>158</v>
+        <v>152</v>
       </c>
       <c r="F96" s="11" t="s">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="G96" s="11" t="s">
         <v>16</v>
@@ -5184,19 +5182,19 @@
       <c r="AE96" s="9"/>
       <c r="AF96" s="9"/>
     </row>
-    <row r="97" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A97" s="9"/>
       <c r="B97" s="9"/>
       <c r="C97" s="9"/>
       <c r="D97" s="9"/>
       <c r="E97" s="10" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="F97" s="11" t="s">
-        <v>157</v>
+        <v>162</v>
       </c>
       <c r="G97" s="11" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H97" s="11" t="s">
         <v>10</v>
@@ -5226,100 +5224,100 @@
       <c r="AE97" s="9"/>
       <c r="AF97" s="9"/>
     </row>
-    <row r="98" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A98" s="9"/>
-      <c r="B98" s="9"/>
-      <c r="C98" s="9"/>
-      <c r="D98" s="9"/>
-      <c r="E98" s="10" t="s">
-        <v>158</v>
-      </c>
-      <c r="F98" s="11" t="s">
-        <v>166</v>
-      </c>
-      <c r="G98" s="11" t="s">
+    <row r="98" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="4"/>
+      <c r="B98" s="4"/>
+      <c r="C98" s="4"/>
+      <c r="D98" s="4"/>
+      <c r="E98" s="13" t="s">
+        <v>156</v>
+      </c>
+      <c r="F98" s="8" t="s">
+        <v>146</v>
+      </c>
+      <c r="G98" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H98" s="11" t="s">
+      <c r="H98" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="I98" s="9"/>
-      <c r="J98" s="9"/>
-      <c r="K98" s="9"/>
-      <c r="L98" s="9"/>
-      <c r="M98" s="9"/>
-      <c r="N98" s="9"/>
-      <c r="O98" s="9"/>
-      <c r="P98" s="9"/>
-      <c r="Q98" s="9"/>
-      <c r="R98" s="9"/>
-      <c r="S98" s="9"/>
-      <c r="T98" s="9"/>
-      <c r="U98" s="9"/>
-      <c r="V98" s="9"/>
-      <c r="W98" s="9"/>
-      <c r="X98" s="9"/>
-      <c r="Y98" s="9"/>
-      <c r="Z98" s="9"/>
-      <c r="AA98" s="9"/>
-      <c r="AB98" s="9"/>
-      <c r="AC98" s="9"/>
-      <c r="AD98" s="9"/>
-      <c r="AE98" s="9"/>
-      <c r="AF98" s="9"/>
-    </row>
-    <row r="99" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="4"/>
-      <c r="B99" s="4"/>
-      <c r="C99" s="4"/>
-      <c r="D99" s="4"/>
-      <c r="E99" s="13" t="s">
-        <v>160</v>
-      </c>
-      <c r="F99" s="8" t="s">
-        <v>150</v>
-      </c>
-      <c r="G99" s="8" t="s">
+      <c r="I98" s="4"/>
+      <c r="J98" s="4"/>
+      <c r="K98" s="4"/>
+      <c r="L98" s="4"/>
+      <c r="M98" s="4"/>
+      <c r="N98" s="4"/>
+      <c r="O98" s="4"/>
+      <c r="P98" s="4"/>
+      <c r="Q98" s="4"/>
+      <c r="R98" s="4"/>
+      <c r="S98" s="4"/>
+      <c r="T98" s="4"/>
+      <c r="U98" s="4"/>
+      <c r="V98" s="4"/>
+      <c r="W98" s="4"/>
+      <c r="X98" s="4"/>
+      <c r="Y98" s="4"/>
+      <c r="Z98" s="4"/>
+      <c r="AA98" s="4"/>
+      <c r="AB98" s="4"/>
+      <c r="AC98" s="4"/>
+      <c r="AD98" s="4"/>
+      <c r="AE98" s="4"/>
+      <c r="AF98" s="4"/>
+    </row>
+    <row r="99" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A99" s="9"/>
+      <c r="B99" s="9"/>
+      <c r="C99" s="9"/>
+      <c r="D99" s="9"/>
+      <c r="E99" s="10" t="s">
+        <v>157</v>
+      </c>
+      <c r="F99" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="G99" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H99" s="8" t="s">
+      <c r="H99" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="I99" s="4"/>
-      <c r="J99" s="4"/>
-      <c r="K99" s="4"/>
-      <c r="L99" s="4"/>
-      <c r="M99" s="4"/>
-      <c r="N99" s="4"/>
-      <c r="O99" s="4"/>
-      <c r="P99" s="4"/>
-      <c r="Q99" s="4"/>
-      <c r="R99" s="4"/>
-      <c r="S99" s="4"/>
-      <c r="T99" s="4"/>
-      <c r="U99" s="4"/>
-      <c r="V99" s="4"/>
-      <c r="W99" s="4"/>
-      <c r="X99" s="4"/>
-      <c r="Y99" s="4"/>
-      <c r="Z99" s="4"/>
-      <c r="AA99" s="4"/>
-      <c r="AB99" s="4"/>
-      <c r="AC99" s="4"/>
-      <c r="AD99" s="4"/>
-      <c r="AE99" s="4"/>
-      <c r="AF99" s="4"/>
-    </row>
-    <row r="100" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I99" s="9"/>
+      <c r="J99" s="9"/>
+      <c r="K99" s="9"/>
+      <c r="L99" s="9"/>
+      <c r="M99" s="9"/>
+      <c r="N99" s="9"/>
+      <c r="O99" s="9"/>
+      <c r="P99" s="9"/>
+      <c r="Q99" s="9"/>
+      <c r="R99" s="9"/>
+      <c r="S99" s="9"/>
+      <c r="T99" s="9"/>
+      <c r="U99" s="9"/>
+      <c r="V99" s="9"/>
+      <c r="W99" s="9"/>
+      <c r="X99" s="9"/>
+      <c r="Y99" s="9"/>
+      <c r="Z99" s="9"/>
+      <c r="AA99" s="9"/>
+      <c r="AB99" s="9"/>
+      <c r="AC99" s="9"/>
+      <c r="AD99" s="9"/>
+      <c r="AE99" s="9"/>
+      <c r="AF99" s="9"/>
+    </row>
+    <row r="100" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A100" s="9"/>
       <c r="B100" s="9"/>
       <c r="C100" s="9"/>
       <c r="D100" s="9"/>
       <c r="E100" s="10" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
       <c r="F100" s="11" t="s">
-        <v>151</v>
+        <v>159</v>
       </c>
       <c r="G100" s="11" t="s">
         <v>9</v>
@@ -5352,16 +5350,16 @@
       <c r="AE100" s="9"/>
       <c r="AF100" s="9"/>
     </row>
-    <row r="101" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A101" s="9"/>
       <c r="B101" s="9"/>
       <c r="C101" s="9"/>
       <c r="D101" s="9"/>
       <c r="E101" s="10" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="F101" s="11" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="G101" s="11" t="s">
         <v>9</v>
@@ -5394,89 +5392,89 @@
       <c r="AE101" s="9"/>
       <c r="AF101" s="9"/>
     </row>
-    <row r="102" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A102" s="9"/>
-      <c r="B102" s="9"/>
-      <c r="C102" s="9"/>
-      <c r="D102" s="9"/>
-      <c r="E102" s="10" t="s">
+    <row r="102" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A102" s="4"/>
+      <c r="B102" s="4"/>
+      <c r="C102" s="4"/>
+      <c r="D102" s="4"/>
+      <c r="E102" s="13" t="s">
+        <v>166</v>
+      </c>
+      <c r="F102" s="8" t="s">
+        <v>163</v>
+      </c>
+      <c r="G102" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="H102" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="I102" s="4"/>
+      <c r="J102" s="4"/>
+      <c r="K102" s="4"/>
+      <c r="L102" s="4"/>
+      <c r="M102" s="4"/>
+      <c r="N102" s="4"/>
+      <c r="O102" s="4"/>
+      <c r="P102" s="4"/>
+      <c r="Q102" s="4"/>
+      <c r="R102" s="4"/>
+      <c r="S102" s="4"/>
+      <c r="T102" s="4"/>
+      <c r="U102" s="4"/>
+      <c r="V102" s="4"/>
+      <c r="W102" s="4"/>
+      <c r="X102" s="4"/>
+      <c r="Y102" s="4"/>
+      <c r="Z102" s="4"/>
+      <c r="AA102" s="4"/>
+      <c r="AB102" s="4"/>
+      <c r="AC102" s="4"/>
+      <c r="AD102" s="4"/>
+      <c r="AE102" s="4"/>
+      <c r="AF102" s="4"/>
+    </row>
+    <row r="103" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A103" s="9"/>
+      <c r="B103" s="9"/>
+      <c r="C103" s="9"/>
+      <c r="D103" s="9"/>
+      <c r="E103" s="10" t="s">
+        <v>167</v>
+      </c>
+      <c r="F103" s="11" t="s">
         <v>164</v>
       </c>
-      <c r="F102" s="11" t="s">
-        <v>165</v>
-      </c>
-      <c r="G102" s="11" t="s">
+      <c r="G103" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H102" s="11" t="s">
-        <v>10</v>
-      </c>
-      <c r="I102" s="9"/>
-      <c r="J102" s="9"/>
-      <c r="K102" s="9"/>
-      <c r="L102" s="9"/>
-      <c r="M102" s="9"/>
-      <c r="N102" s="9"/>
-      <c r="O102" s="9"/>
-      <c r="P102" s="9"/>
-      <c r="Q102" s="9"/>
-      <c r="R102" s="9"/>
-      <c r="S102" s="9"/>
-      <c r="T102" s="9"/>
-      <c r="U102" s="9"/>
-      <c r="V102" s="9"/>
-      <c r="W102" s="9"/>
-      <c r="X102" s="9"/>
-      <c r="Y102" s="9"/>
-      <c r="Z102" s="9"/>
-      <c r="AA102" s="9"/>
-      <c r="AB102" s="9"/>
-      <c r="AC102" s="9"/>
-      <c r="AD102" s="9"/>
-      <c r="AE102" s="9"/>
-      <c r="AF102" s="9"/>
-    </row>
-    <row r="103" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A103" s="4"/>
-      <c r="B103" s="4"/>
-      <c r="C103" s="4"/>
-      <c r="D103" s="4"/>
-      <c r="E103" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="F103" s="8" t="s">
-        <v>167</v>
-      </c>
-      <c r="G103" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="H103" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="I103" s="4"/>
-      <c r="J103" s="4"/>
-      <c r="K103" s="4"/>
-      <c r="L103" s="4"/>
-      <c r="M103" s="4"/>
-      <c r="N103" s="4"/>
-      <c r="O103" s="4"/>
-      <c r="P103" s="4"/>
-      <c r="Q103" s="4"/>
-      <c r="R103" s="4"/>
-      <c r="S103" s="4"/>
-      <c r="T103" s="4"/>
-      <c r="U103" s="4"/>
-      <c r="V103" s="4"/>
-      <c r="W103" s="4"/>
-      <c r="X103" s="4"/>
-      <c r="Y103" s="4"/>
-      <c r="Z103" s="4"/>
-      <c r="AA103" s="4"/>
-      <c r="AB103" s="4"/>
-      <c r="AC103" s="4"/>
-      <c r="AD103" s="4"/>
-      <c r="AE103" s="4"/>
-      <c r="AF103" s="4"/>
+      <c r="H103" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="I103" s="9"/>
+      <c r="J103" s="9"/>
+      <c r="K103" s="9"/>
+      <c r="L103" s="9"/>
+      <c r="M103" s="9"/>
+      <c r="N103" s="9"/>
+      <c r="O103" s="9"/>
+      <c r="P103" s="9"/>
+      <c r="Q103" s="9"/>
+      <c r="R103" s="9"/>
+      <c r="S103" s="9"/>
+      <c r="T103" s="9"/>
+      <c r="U103" s="9"/>
+      <c r="V103" s="9"/>
+      <c r="W103" s="9"/>
+      <c r="X103" s="9"/>
+      <c r="Y103" s="9"/>
+      <c r="Z103" s="9"/>
+      <c r="AA103" s="9"/>
+      <c r="AB103" s="9"/>
+      <c r="AC103" s="9"/>
+      <c r="AD103" s="9"/>
+      <c r="AE103" s="9"/>
+      <c r="AF103" s="9"/>
     </row>
     <row r="104" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A104" s="9"/>
@@ -5484,16 +5482,16 @@
       <c r="C104" s="9"/>
       <c r="D104" s="9"/>
       <c r="E104" s="10" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F104" s="11" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="G104" s="11" t="s">
         <v>9</v>
       </c>
       <c r="H104" s="11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="I104" s="9"/>
       <c r="J104" s="9"/>
@@ -5525,16 +5523,16 @@
       <c r="B105" s="9"/>
       <c r="C105" s="9"/>
       <c r="D105" s="9"/>
-      <c r="E105" s="10" t="s">
-        <v>172</v>
-      </c>
-      <c r="F105" s="11" t="s">
-        <v>169</v>
-      </c>
-      <c r="G105" s="11" t="s">
+      <c r="E105" s="13" t="s">
+        <v>171</v>
+      </c>
+      <c r="F105" s="8" t="s">
+        <v>170</v>
+      </c>
+      <c r="G105" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="H105" s="11" t="s">
+      <c r="H105" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I105" s="9"/>
@@ -5567,16 +5565,16 @@
       <c r="B106" s="9"/>
       <c r="C106" s="9"/>
       <c r="D106" s="9"/>
-      <c r="E106" s="13" t="s">
-        <v>175</v>
-      </c>
-      <c r="F106" s="8" t="s">
-        <v>174</v>
-      </c>
-      <c r="G106" s="8" t="s">
+      <c r="E106" s="10" t="s">
+        <v>173</v>
+      </c>
+      <c r="F106" s="11" t="s">
+        <v>198</v>
+      </c>
+      <c r="G106" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="H106" s="8" t="s">
+      <c r="H106" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I106" s="9"/>
@@ -5610,10 +5608,10 @@
       <c r="C107" s="9"/>
       <c r="D107" s="9"/>
       <c r="E107" s="10" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="F107" s="11" t="s">
-        <v>202</v>
+        <v>199</v>
       </c>
       <c r="G107" s="11" t="s">
         <v>9</v>
@@ -5652,10 +5650,10 @@
       <c r="C108" s="9"/>
       <c r="D108" s="9"/>
       <c r="E108" s="10" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
       <c r="F108" s="11" t="s">
-        <v>203</v>
+        <v>200</v>
       </c>
       <c r="G108" s="11" t="s">
         <v>9</v>
@@ -5694,13 +5692,13 @@
       <c r="C109" s="9"/>
       <c r="D109" s="9"/>
       <c r="E109" s="10" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="F109" s="11" t="s">
-        <v>204</v>
+        <v>175</v>
       </c>
       <c r="G109" s="11" t="s">
-        <v>9</v>
+        <v>17</v>
       </c>
       <c r="H109" s="11" t="s">
         <v>10</v>
@@ -5736,13 +5734,13 @@
       <c r="C110" s="9"/>
       <c r="D110" s="9"/>
       <c r="E110" s="10" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="F110" s="11" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="G110" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H110" s="11" t="s">
         <v>10</v>
@@ -5778,10 +5776,10 @@
       <c r="C111" s="9"/>
       <c r="D111" s="9"/>
       <c r="E111" s="10" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="F111" s="11" t="s">
-        <v>180</v>
+        <v>197</v>
       </c>
       <c r="G111" s="11" t="s">
         <v>16</v>
@@ -5820,13 +5818,13 @@
       <c r="C112" s="9"/>
       <c r="D112" s="9"/>
       <c r="E112" s="10" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="F112" s="11" t="s">
-        <v>201</v>
+        <v>177</v>
       </c>
       <c r="G112" s="11" t="s">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="H112" s="11" t="s">
         <v>10</v>
@@ -5862,10 +5860,10 @@
       <c r="C113" s="9"/>
       <c r="D113" s="9"/>
       <c r="E113" s="10" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
       <c r="F113" s="11" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="G113" s="11" t="s">
         <v>9</v>
@@ -5904,10 +5902,10 @@
       <c r="C114" s="9"/>
       <c r="D114" s="9"/>
       <c r="E114" s="10" t="s">
+        <v>186</v>
+      </c>
+      <c r="F114" s="11" t="s">
         <v>189</v>
-      </c>
-      <c r="F114" s="11" t="s">
-        <v>182</v>
       </c>
       <c r="G114" s="11" t="s">
         <v>9</v>
@@ -5946,10 +5944,10 @@
       <c r="C115" s="9"/>
       <c r="D115" s="9"/>
       <c r="E115" s="10" t="s">
-        <v>190</v>
+        <v>187</v>
       </c>
       <c r="F115" s="11" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="G115" s="11" t="s">
         <v>9</v>
@@ -5988,10 +5986,10 @@
       <c r="C116" s="9"/>
       <c r="D116" s="9"/>
       <c r="E116" s="10" t="s">
-        <v>191</v>
+        <v>193</v>
       </c>
       <c r="F116" s="11" t="s">
-        <v>183</v>
+        <v>188</v>
       </c>
       <c r="G116" s="11" t="s">
         <v>9</v>
@@ -6030,10 +6028,10 @@
       <c r="C117" s="9"/>
       <c r="D117" s="9"/>
       <c r="E117" s="10" t="s">
-        <v>197</v>
+        <v>194</v>
       </c>
       <c r="F117" s="11" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="G117" s="11" t="s">
         <v>9</v>
@@ -6072,10 +6070,10 @@
       <c r="C118" s="9"/>
       <c r="D118" s="9"/>
       <c r="E118" s="10" t="s">
-        <v>198</v>
+        <v>195</v>
       </c>
       <c r="F118" s="11" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="G118" s="11" t="s">
         <v>9</v>
@@ -6114,13 +6112,13 @@
       <c r="C119" s="9"/>
       <c r="D119" s="9"/>
       <c r="E119" s="10" t="s">
-        <v>199</v>
+        <v>196</v>
       </c>
       <c r="F119" s="11" t="s">
-        <v>195</v>
+        <v>192</v>
       </c>
       <c r="G119" s="11" t="s">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="H119" s="11" t="s">
         <v>10</v>
@@ -6155,16 +6153,16 @@
       <c r="B120" s="9"/>
       <c r="C120" s="9"/>
       <c r="D120" s="9"/>
-      <c r="E120" s="10" t="s">
-        <v>200</v>
-      </c>
-      <c r="F120" s="11" t="s">
-        <v>196</v>
-      </c>
-      <c r="G120" s="11" t="s">
+      <c r="E120" s="13" t="s">
+        <v>201</v>
+      </c>
+      <c r="F120" s="8" t="s">
+        <v>172</v>
+      </c>
+      <c r="G120" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H120" s="11" t="s">
+      <c r="H120" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I120" s="9"/>
@@ -6192,22 +6190,22 @@
       <c r="AE120" s="9"/>
       <c r="AF120" s="9"/>
     </row>
-    <row r="121" spans="1:32" s="12" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A121" s="9"/>
       <c r="B121" s="9"/>
       <c r="C121" s="9"/>
       <c r="D121" s="9"/>
-      <c r="E121" s="13" t="s">
-        <v>205</v>
-      </c>
-      <c r="F121" s="8" t="s">
-        <v>176</v>
-      </c>
-      <c r="G121" s="8" t="s">
+      <c r="E121" s="10" t="s">
+        <v>202</v>
+      </c>
+      <c r="F121" s="11" t="s">
+        <v>203</v>
+      </c>
+      <c r="G121" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H121" s="8" t="s">
-        <v>256</v>
+      <c r="H121" s="11" t="s">
+        <v>10</v>
       </c>
       <c r="I121" s="9"/>
       <c r="J121" s="9"/>
@@ -6240,16 +6238,16 @@
       <c r="C122" s="9"/>
       <c r="D122" s="9"/>
       <c r="E122" s="10" t="s">
+        <v>204</v>
+      </c>
+      <c r="F122" s="11" t="s">
         <v>206</v>
-      </c>
-      <c r="F122" s="11" t="s">
-        <v>207</v>
       </c>
       <c r="G122" s="11" t="s">
         <v>16</v>
       </c>
       <c r="H122" s="11" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="I122" s="9"/>
       <c r="J122" s="9"/>
@@ -6276,16 +6274,16 @@
       <c r="AE122" s="9"/>
       <c r="AF122" s="9"/>
     </row>
-    <row r="123" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A123" s="9"/>
       <c r="B123" s="9"/>
       <c r="C123" s="9"/>
       <c r="D123" s="9"/>
       <c r="E123" s="10" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="F123" s="11" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G123" s="11" t="s">
         <v>16</v>
@@ -6318,16 +6316,16 @@
       <c r="AE123" s="9"/>
       <c r="AF123" s="9"/>
     </row>
-    <row r="124" spans="1:32" s="12" customFormat="1" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A124" s="9"/>
       <c r="B124" s="9"/>
       <c r="C124" s="9"/>
       <c r="D124" s="9"/>
       <c r="E124" s="10" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="F124" s="11" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G124" s="11" t="s">
         <v>16</v>
@@ -6360,61 +6358,61 @@
       <c r="AE124" s="9"/>
       <c r="AF124" s="9"/>
     </row>
-    <row r="125" spans="1:32" s="12" customFormat="1" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A125" s="9"/>
-      <c r="B125" s="9"/>
-      <c r="C125" s="9"/>
-      <c r="D125" s="9"/>
-      <c r="E125" s="10" t="s">
-        <v>209</v>
-      </c>
-      <c r="F125" s="11" t="s">
-        <v>212</v>
-      </c>
-      <c r="G125" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H125" s="11" t="s">
-        <v>11</v>
-      </c>
-      <c r="I125" s="9"/>
-      <c r="J125" s="9"/>
-      <c r="K125" s="9"/>
-      <c r="L125" s="9"/>
-      <c r="M125" s="9"/>
-      <c r="N125" s="9"/>
-      <c r="O125" s="9"/>
-      <c r="P125" s="9"/>
-      <c r="Q125" s="9"/>
-      <c r="R125" s="9"/>
-      <c r="S125" s="9"/>
-      <c r="T125" s="9"/>
-      <c r="U125" s="9"/>
-      <c r="V125" s="9"/>
-      <c r="W125" s="9"/>
-      <c r="X125" s="9"/>
-      <c r="Y125" s="9"/>
-      <c r="Z125" s="9"/>
-      <c r="AA125" s="9"/>
-      <c r="AB125" s="9"/>
-      <c r="AC125" s="9"/>
-      <c r="AD125" s="9"/>
-      <c r="AE125" s="9"/>
-      <c r="AF125" s="9"/>
+    <row r="125" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A125" s="4"/>
+      <c r="B125" s="4"/>
+      <c r="C125" s="4"/>
+      <c r="D125" s="4"/>
+      <c r="E125" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="F125" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="G125" s="2"/>
+      <c r="H125" s="2"/>
+      <c r="I125" s="4"/>
+      <c r="J125" s="4"/>
+      <c r="K125" s="4"/>
+      <c r="L125" s="4"/>
+      <c r="M125" s="4"/>
+      <c r="N125" s="4"/>
+      <c r="O125" s="4"/>
+      <c r="P125" s="4"/>
+      <c r="Q125" s="4"/>
+      <c r="R125" s="4"/>
+      <c r="S125" s="4"/>
+      <c r="T125" s="4"/>
+      <c r="U125" s="4"/>
+      <c r="V125" s="4"/>
+      <c r="W125" s="4"/>
+      <c r="X125" s="4"/>
+      <c r="Y125" s="4"/>
+      <c r="Z125" s="4"/>
+      <c r="AA125" s="4"/>
+      <c r="AB125" s="4"/>
+      <c r="AC125" s="4"/>
+      <c r="AD125" s="4"/>
+      <c r="AE125" s="4"/>
+      <c r="AF125" s="4"/>
     </row>
     <row r="126" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A126" s="4"/>
       <c r="B126" s="4"/>
       <c r="C126" s="4"/>
       <c r="D126" s="4"/>
-      <c r="E126" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="F126" s="2" t="s">
-        <v>130</v>
-      </c>
-      <c r="G126" s="2"/>
-      <c r="H126" s="2"/>
+      <c r="E126" s="13" t="s">
+        <v>209</v>
+      </c>
+      <c r="F126" s="8" t="s">
+        <v>210</v>
+      </c>
+      <c r="G126" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="H126" s="8" t="s">
+        <v>10</v>
+      </c>
       <c r="I126" s="4"/>
       <c r="J126" s="4"/>
       <c r="K126" s="4"/>
@@ -6445,16 +6443,16 @@
       <c r="B127" s="4"/>
       <c r="C127" s="4"/>
       <c r="D127" s="4"/>
-      <c r="E127" s="13" t="s">
-        <v>213</v>
-      </c>
-      <c r="F127" s="8" t="s">
-        <v>214</v>
-      </c>
-      <c r="G127" s="8" t="s">
+      <c r="E127" s="10" t="s">
+        <v>211</v>
+      </c>
+      <c r="F127" s="11" t="s">
+        <v>268</v>
+      </c>
+      <c r="G127" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H127" s="8" t="s">
+      <c r="H127" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I127" s="4"/>
@@ -6488,10 +6486,10 @@
       <c r="C128" s="4"/>
       <c r="D128" s="4"/>
       <c r="E128" s="10" t="s">
-        <v>215</v>
+        <v>219</v>
       </c>
       <c r="F128" s="11" t="s">
-        <v>216</v>
+        <v>269</v>
       </c>
       <c r="G128" s="11" t="s">
         <v>16</v>
@@ -6530,10 +6528,10 @@
       <c r="C129" s="4"/>
       <c r="D129" s="4"/>
       <c r="E129" s="10" t="s">
-        <v>226</v>
+        <v>220</v>
       </c>
       <c r="F129" s="11" t="s">
-        <v>217</v>
+        <v>270</v>
       </c>
       <c r="G129" s="11" t="s">
         <v>16</v>
@@ -6572,13 +6570,13 @@
       <c r="C130" s="4"/>
       <c r="D130" s="4"/>
       <c r="E130" s="10" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="F130" s="11" t="s">
-        <v>218</v>
+        <v>215</v>
       </c>
       <c r="G130" s="11" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="H130" s="11" t="s">
         <v>10</v>
@@ -6614,10 +6612,10 @@
       <c r="C131" s="4"/>
       <c r="D131" s="4"/>
       <c r="E131" s="10" t="s">
-        <v>228</v>
+        <v>222</v>
       </c>
       <c r="F131" s="11" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G131" s="11" t="s">
         <v>17</v>
@@ -6656,10 +6654,10 @@
       <c r="C132" s="4"/>
       <c r="D132" s="4"/>
       <c r="E132" s="10" t="s">
-        <v>229</v>
+        <v>223</v>
       </c>
       <c r="F132" s="11" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="G132" s="11" t="s">
         <v>17</v>
@@ -6692,19 +6690,19 @@
       <c r="AE132" s="4"/>
       <c r="AF132" s="4"/>
     </row>
-    <row r="133" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A133" s="4"/>
       <c r="B133" s="4"/>
       <c r="C133" s="4"/>
       <c r="D133" s="4"/>
       <c r="E133" s="10" t="s">
-        <v>230</v>
+        <v>224</v>
       </c>
       <c r="F133" s="11" t="s">
-        <v>224</v>
+        <v>218</v>
       </c>
       <c r="G133" s="11" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="H133" s="11" t="s">
         <v>10</v>
@@ -6734,21 +6732,21 @@
       <c r="AE133" s="4"/>
       <c r="AF133" s="4"/>
     </row>
-    <row r="134" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A134" s="4"/>
       <c r="B134" s="4"/>
       <c r="C134" s="4"/>
       <c r="D134" s="4"/>
-      <c r="E134" s="10" t="s">
-        <v>231</v>
-      </c>
-      <c r="F134" s="11" t="s">
-        <v>225</v>
-      </c>
-      <c r="G134" s="11" t="s">
+      <c r="E134" s="13" t="s">
+        <v>243</v>
+      </c>
+      <c r="F134" s="8" t="s">
+        <v>242</v>
+      </c>
+      <c r="G134" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="H134" s="11" t="s">
+      <c r="H134" s="8" t="s">
         <v>10</v>
       </c>
       <c r="I134" s="4"/>
@@ -6776,21 +6774,21 @@
       <c r="AE134" s="4"/>
       <c r="AF134" s="4"/>
     </row>
-    <row r="135" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A135" s="4"/>
       <c r="B135" s="4"/>
       <c r="C135" s="4"/>
       <c r="D135" s="4"/>
-      <c r="E135" s="13" t="s">
-        <v>258</v>
-      </c>
-      <c r="F135" s="8" t="s">
-        <v>257</v>
-      </c>
-      <c r="G135" s="8" t="s">
+      <c r="E135" s="10" t="s">
+        <v>244</v>
+      </c>
+      <c r="F135" s="11" t="s">
+        <v>245</v>
+      </c>
+      <c r="G135" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="H135" s="8" t="s">
+      <c r="H135" s="11" t="s">
         <v>10</v>
       </c>
       <c r="I135" s="4"/>
@@ -6824,10 +6822,10 @@
       <c r="C136" s="4"/>
       <c r="D136" s="4"/>
       <c r="E136" s="10" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="F136" s="11" t="s">
-        <v>260</v>
+        <v>248</v>
       </c>
       <c r="G136" s="11" t="s">
         <v>16</v>
@@ -6860,16 +6858,16 @@
       <c r="AE136" s="4"/>
       <c r="AF136" s="4"/>
     </row>
-    <row r="137" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A137" s="4"/>
       <c r="B137" s="4"/>
       <c r="C137" s="4"/>
       <c r="D137" s="4"/>
       <c r="E137" s="10" t="s">
-        <v>261</v>
+        <v>247</v>
       </c>
       <c r="F137" s="11" t="s">
-        <v>263</v>
+        <v>249</v>
       </c>
       <c r="G137" s="11" t="s">
         <v>16</v>
@@ -6902,16 +6900,16 @@
       <c r="AE137" s="4"/>
       <c r="AF137" s="4"/>
     </row>
-    <row r="138" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A138" s="4"/>
       <c r="B138" s="4"/>
       <c r="C138" s="4"/>
       <c r="D138" s="4"/>
       <c r="E138" s="10" t="s">
-        <v>262</v>
+        <v>250</v>
       </c>
       <c r="F138" s="11" t="s">
-        <v>264</v>
+        <v>253</v>
       </c>
       <c r="G138" s="11" t="s">
         <v>16</v>
@@ -6944,16 +6942,16 @@
       <c r="AE138" s="4"/>
       <c r="AF138" s="4"/>
     </row>
-    <row r="139" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A139" s="4"/>
       <c r="B139" s="4"/>
       <c r="C139" s="4"/>
       <c r="D139" s="4"/>
       <c r="E139" s="10" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="F139" s="11" t="s">
-        <v>268</v>
+        <v>252</v>
       </c>
       <c r="G139" s="11" t="s">
         <v>16</v>
@@ -6992,10 +6990,10 @@
       <c r="C140" s="4"/>
       <c r="D140" s="4"/>
       <c r="E140" s="10" t="s">
-        <v>266</v>
+        <v>250</v>
       </c>
       <c r="F140" s="11" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="G140" s="11" t="s">
         <v>16</v>
@@ -7028,16 +7026,16 @@
       <c r="AE140" s="4"/>
       <c r="AF140" s="4"/>
     </row>
-    <row r="141" spans="1:32" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A141" s="4"/>
       <c r="B141" s="4"/>
       <c r="C141" s="4"/>
       <c r="D141" s="4"/>
       <c r="E141" s="10" t="s">
-        <v>265</v>
+        <v>251</v>
       </c>
       <c r="F141" s="11" t="s">
-        <v>269</v>
+        <v>257</v>
       </c>
       <c r="G141" s="11" t="s">
         <v>16</v>
@@ -7070,23 +7068,15 @@
       <c r="AE141" s="4"/>
       <c r="AF141" s="4"/>
     </row>
-    <row r="142" spans="1:32" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A142" s="4"/>
       <c r="B142" s="4"/>
       <c r="C142" s="4"/>
       <c r="D142" s="4"/>
-      <c r="E142" s="10" t="s">
-        <v>266</v>
-      </c>
-      <c r="F142" s="11" t="s">
-        <v>272</v>
-      </c>
-      <c r="G142" s="11" t="s">
-        <v>16</v>
-      </c>
-      <c r="H142" s="11" t="s">
-        <v>10</v>
-      </c>
+      <c r="E142" s="4"/>
+      <c r="F142" s="4"/>
+      <c r="G142" s="4"/>
+      <c r="H142" s="4"/>
       <c r="I142" s="4"/>
       <c r="J142" s="4"/>
       <c r="K142" s="4"/>
@@ -7146,13 +7136,15 @@
       <c r="AE143" s="4"/>
       <c r="AF143" s="4"/>
     </row>
-    <row r="144" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="4"/>
       <c r="B144" s="4"/>
       <c r="C144" s="4"/>
       <c r="D144" s="4"/>
-      <c r="E144" s="4"/>
-      <c r="F144" s="4"/>
+      <c r="E144" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="F144" s="7"/>
       <c r="G144" s="4"/>
       <c r="H144" s="4"/>
       <c r="I144" s="4"/>
@@ -7186,7 +7178,7 @@
       <c r="C145" s="4"/>
       <c r="D145" s="4"/>
       <c r="E145" s="6" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="F145" s="7"/>
       <c r="G145" s="4"/>
@@ -7222,7 +7214,7 @@
       <c r="C146" s="4"/>
       <c r="D146" s="4"/>
       <c r="E146" s="6" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="F146" s="7"/>
       <c r="G146" s="4"/>
@@ -7258,7 +7250,7 @@
       <c r="C147" s="4"/>
       <c r="D147" s="4"/>
       <c r="E147" s="6" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="F147" s="7"/>
       <c r="G147" s="4"/>
@@ -7288,15 +7280,13 @@
       <c r="AE147" s="4"/>
       <c r="AF147" s="4"/>
     </row>
-    <row r="148" spans="1:32" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A148" s="4"/>
       <c r="B148" s="4"/>
       <c r="C148" s="4"/>
       <c r="D148" s="4"/>
-      <c r="E148" s="6" t="s">
-        <v>6</v>
-      </c>
-      <c r="F148" s="7"/>
+      <c r="E148" s="4"/>
+      <c r="F148" s="4"/>
       <c r="G148" s="4"/>
       <c r="H148" s="4"/>
       <c r="I148" s="4"/>
@@ -10554,40 +10544,6 @@
       <c r="AE243" s="4"/>
       <c r="AF243" s="4"/>
     </row>
-    <row r="244" spans="1:32" x14ac:dyDescent="0.25">
-      <c r="A244" s="4"/>
-      <c r="B244" s="4"/>
-      <c r="C244" s="4"/>
-      <c r="D244" s="4"/>
-      <c r="E244" s="4"/>
-      <c r="F244" s="4"/>
-      <c r="G244" s="4"/>
-      <c r="H244" s="4"/>
-      <c r="I244" s="4"/>
-      <c r="J244" s="4"/>
-      <c r="K244" s="4"/>
-      <c r="L244" s="4"/>
-      <c r="M244" s="4"/>
-      <c r="N244" s="4"/>
-      <c r="O244" s="4"/>
-      <c r="P244" s="4"/>
-      <c r="Q244" s="4"/>
-      <c r="R244" s="4"/>
-      <c r="S244" s="4"/>
-      <c r="T244" s="4"/>
-      <c r="U244" s="4"/>
-      <c r="V244" s="4"/>
-      <c r="W244" s="4"/>
-      <c r="X244" s="4"/>
-      <c r="Y244" s="4"/>
-      <c r="Z244" s="4"/>
-      <c r="AA244" s="4"/>
-      <c r="AB244" s="4"/>
-      <c r="AC244" s="4"/>
-      <c r="AD244" s="4"/>
-      <c r="AE244" s="4"/>
-      <c r="AF244" s="4"/>
-    </row>
   </sheetData>
   <mergeCells count="4">
     <mergeCell ref="E8:E9"/>
@@ -10598,10 +10554,10 @@
   <hyperlinks>
     <hyperlink ref="E8" location="_ftn1" display="_ftn1"/>
     <hyperlink ref="F8" location="_ftn2" display="_ftn2"/>
-    <hyperlink ref="E148" location="_ftnref4" display="_ftnref4"/>
-    <hyperlink ref="E147" location="_ftnref3" display="_ftnref3"/>
-    <hyperlink ref="E146" location="_ftnref2" display="_ftnref2"/>
-    <hyperlink ref="E145" location="_ftnref1" display="_ftnref1"/>
+    <hyperlink ref="E147" location="_ftnref4" display="_ftnref4"/>
+    <hyperlink ref="E146" location="_ftnref3" display="_ftnref3"/>
+    <hyperlink ref="E145" location="_ftnref2" display="_ftnref2"/>
+    <hyperlink ref="E144" location="_ftnref1" display="_ftnref1"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" r:id="rId1"/>

</xml_diff>